<commit_message>
added duck data, updating card styling
</commit_message>
<xml_diff>
--- a/data/duck_data.xlsx
+++ b/data/duck_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\Documents\DS_Projects\portfolio-deployments\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28CCD1A-839D-46BC-9087-B334D012CA1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E6EEA9-2D26-4D15-B9BC-EDEDA8AA5788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EF9DEEC2-186D-4161-AB80-57C24753F6AE}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15750" xr2:uid="{EF9DEEC2-186D-4161-AB80-57C24753F6AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Ducks" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="454">
   <si>
     <t>Duck</t>
   </si>
@@ -1390,6 +1390,42 @@
   </si>
   <si>
     <t>Frau Blücher  ⚡⚡⚡</t>
+  </si>
+  <si>
+    <t>shark</t>
+  </si>
+  <si>
+    <t>beach sunglass blue</t>
+  </si>
+  <si>
+    <t>Anchors</t>
+  </si>
+  <si>
+    <t>Octopi</t>
+  </si>
+  <si>
+    <t>Captain w glasses</t>
+  </si>
+  <si>
+    <t>Bucky's</t>
+  </si>
+  <si>
+    <t>Universal Studios</t>
+  </si>
+  <si>
+    <t>Derek &amp; Cassi</t>
+  </si>
+  <si>
+    <t>Orlando</t>
+  </si>
+  <si>
+    <t>The Boathouse</t>
+  </si>
+  <si>
+    <t>Lake Buena Vista</t>
+  </si>
+  <si>
+    <t>Buc-ee's</t>
   </si>
 </sst>
 </file>
@@ -1479,6 +1515,9 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1514,9 +1553,6 @@
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1531,8 +1567,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55715085-9AFB-4516-817F-DC3F49C2B133}" name="Table1" displayName="Table1" ref="A1:R119" totalsRowShown="0">
-  <autoFilter ref="A1:R119" xr:uid="{55715085-9AFB-4516-817F-DC3F49C2B133}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55715085-9AFB-4516-817F-DC3F49C2B133}" name="Table1" displayName="Table1" ref="A1:R126" totalsRowShown="0">
+  <autoFilter ref="A1:R126" xr:uid="{55715085-9AFB-4516-817F-DC3F49C2B133}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R98">
     <sortCondition ref="I1:I98"/>
   </sortState>
@@ -1545,10 +1581,10 @@
     <tableColumn id="18" xr3:uid="{6CF5BE57-FA6C-4A82-BBEB-02BD6F0FF1A7}" name="Purchase_State"/>
     <tableColumn id="16" xr3:uid="{8F6D77DD-9950-4A0C-9650-EF78F2440AF5}" name="Purchase_Country"/>
     <tableColumn id="17" xr3:uid="{53E3F17B-A5D5-4AE9-83A1-0970087FA2AC}" name="ISO_Code"/>
-    <tableColumn id="4" xr3:uid="{3483BEC1-7940-46EA-87AB-895F2A60F5C4}" name="Date_Bought" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{DD5702CA-A5AA-48F2-A221-5B11E7770312}" name="Latitude" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{6E84405B-586B-45AE-8AAB-E75DDE55DE14}" name="Longitude" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{D54F7BD0-C645-4075-B34E-4D059919801A}" name="About Me" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{3483BEC1-7940-46EA-87AB-895F2A60F5C4}" name="Date_Bought" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{DD5702CA-A5AA-48F2-A221-5B11E7770312}" name="Latitude" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{6E84405B-586B-45AE-8AAB-E75DDE55DE14}" name="Longitude" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{D54F7BD0-C645-4075-B34E-4D059919801A}" name="About Me" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{E6929EE2-9995-48C5-99C7-C33245F8F30B}" name="Buyer"/>
     <tableColumn id="8" xr3:uid="{291141F9-BF51-4E10-B8D7-FD40E791433E}" name="Quantity"/>
     <tableColumn id="9" xr3:uid="{B5508D8E-FAD5-4D52-8444-0DB243E6A995}" name="Total_Weight"/>
@@ -1567,7 +1603,7 @@
     <tableColumn id="1" xr3:uid="{9E64D190-0A43-40CF-AD36-FD04A662496B}" name="Cousins"/>
     <tableColumn id="2" xr3:uid="{B24B008B-4FA5-4F53-8DFF-6B5E687E43FD}" name="Description"/>
     <tableColumn id="3" xr3:uid="{D04918B6-CEB1-4249-B203-04B49B77C2DB}" name="Location bought"/>
-    <tableColumn id="4" xr3:uid="{3D940517-F53B-4DDA-9410-4146A9DBC72B}" name="Date Bought" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{3D940517-F53B-4DDA-9410-4146A9DBC72B}" name="Date Bought" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{51611A3A-347A-410D-87A5-C3B9A034AE16}" name="Fun Fact?"/>
     <tableColumn id="6" xr3:uid="{148B1608-FB51-4737-AD44-B59CA6A1087F}" name="Bought By"/>
     <tableColumn id="7" xr3:uid="{F988032F-024C-44D8-A1BB-16110E5DAE33}" name="Catch Phrase"/>
@@ -1579,9 +1615,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1619,7 +1655,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1725,7 +1761,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1867,7 +1903,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1875,11 +1911,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28BE0B7-C424-43DE-B13E-D21D7F7285C7}">
-  <dimension ref="A1:V119"/>
+  <dimension ref="A1:V126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="67" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="67" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C108" sqref="C108"/>
+      <selection pane="topRight" activeCell="L110" sqref="L110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1888,15 +1924,15 @@
     <col min="2" max="2" width="27.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="39.88671875" customWidth="1"/>
-    <col min="13" max="13" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.6640625" bestFit="1" customWidth="1"/>
@@ -8682,6 +8718,412 @@
       <c r="R119">
         <f>1+6/16</f>
         <v>1.375</v>
+      </c>
+    </row>
+    <row r="120" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>442</v>
+      </c>
+      <c r="B120">
+        <v>30</v>
+      </c>
+      <c r="C120" t="s">
+        <v>420</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E120" t="s">
+        <v>327</v>
+      </c>
+      <c r="F120" t="s">
+        <v>163</v>
+      </c>
+      <c r="G120" t="s">
+        <v>146</v>
+      </c>
+      <c r="H120" t="s">
+        <v>146</v>
+      </c>
+      <c r="I120" s="1">
+        <v>45383</v>
+      </c>
+      <c r="J120" s="4">
+        <v>39.056086162518199</v>
+      </c>
+      <c r="K120" s="4">
+        <v>-77.114897400000004</v>
+      </c>
+      <c r="L120" s="6">
+        <v>46</v>
+      </c>
+      <c r="M120" t="s">
+        <v>50</v>
+      </c>
+      <c r="N120">
+        <v>1</v>
+      </c>
+      <c r="O120">
+        <v>28</v>
+      </c>
+      <c r="P120">
+        <f>2+10/16</f>
+        <v>2.625</v>
+      </c>
+      <c r="Q120">
+        <v>2.25</v>
+      </c>
+      <c r="R120">
+        <f>2+15/16</f>
+        <v>2.9375</v>
+      </c>
+    </row>
+    <row r="121" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>443</v>
+      </c>
+      <c r="B121">
+        <v>31</v>
+      </c>
+      <c r="C121" t="s">
+        <v>420</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E121" t="s">
+        <v>327</v>
+      </c>
+      <c r="F121" t="s">
+        <v>163</v>
+      </c>
+      <c r="G121" t="s">
+        <v>146</v>
+      </c>
+      <c r="H121" t="s">
+        <v>146</v>
+      </c>
+      <c r="I121" s="1">
+        <v>45383</v>
+      </c>
+      <c r="J121" s="4">
+        <v>39.056086162518199</v>
+      </c>
+      <c r="K121" s="4">
+        <v>-77.114897400000004</v>
+      </c>
+      <c r="L121" s="6">
+        <v>47</v>
+      </c>
+      <c r="M121" t="s">
+        <v>50</v>
+      </c>
+      <c r="N121">
+        <v>1</v>
+      </c>
+      <c r="O121">
+        <v>27</v>
+      </c>
+      <c r="P121">
+        <v>2.25</v>
+      </c>
+      <c r="Q121">
+        <f>2+3/16</f>
+        <v>2.1875</v>
+      </c>
+      <c r="R121">
+        <f>2+6/16</f>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="122" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>444</v>
+      </c>
+      <c r="B122">
+        <v>32</v>
+      </c>
+      <c r="C122" t="s">
+        <v>420</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="E122" t="s">
+        <v>452</v>
+      </c>
+      <c r="F122" t="s">
+        <v>167</v>
+      </c>
+      <c r="G122" t="s">
+        <v>146</v>
+      </c>
+      <c r="H122" t="s">
+        <v>146</v>
+      </c>
+      <c r="I122" s="1">
+        <v>45407</v>
+      </c>
+      <c r="J122" s="4">
+        <v>28.371808918683801</v>
+      </c>
+      <c r="K122" s="4">
+        <v>-81.517879136438097</v>
+      </c>
+      <c r="L122" s="6">
+        <v>48</v>
+      </c>
+      <c r="M122" t="s">
+        <v>50</v>
+      </c>
+      <c r="N122">
+        <v>1</v>
+      </c>
+      <c r="O122">
+        <v>18</v>
+      </c>
+      <c r="P122">
+        <v>2</v>
+      </c>
+      <c r="Q122">
+        <f>1+10/16</f>
+        <v>1.625</v>
+      </c>
+      <c r="R122">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="123" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>445</v>
+      </c>
+      <c r="B123">
+        <v>33</v>
+      </c>
+      <c r="C123" t="s">
+        <v>131</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="E123" t="s">
+        <v>450</v>
+      </c>
+      <c r="F123" t="s">
+        <v>167</v>
+      </c>
+      <c r="G123" t="s">
+        <v>146</v>
+      </c>
+      <c r="H123" t="s">
+        <v>146</v>
+      </c>
+      <c r="I123" s="1">
+        <v>45403</v>
+      </c>
+      <c r="J123" s="4">
+        <v>28.4809629890139</v>
+      </c>
+      <c r="K123" s="4">
+        <v>-81.467406691372901</v>
+      </c>
+      <c r="L123" s="6">
+        <v>49</v>
+      </c>
+      <c r="M123" t="s">
+        <v>50</v>
+      </c>
+      <c r="N123">
+        <v>2</v>
+      </c>
+      <c r="O123">
+        <v>35</v>
+      </c>
+      <c r="P123">
+        <f>1+10/16</f>
+        <v>1.625</v>
+      </c>
+      <c r="Q123">
+        <f>2+2/16</f>
+        <v>2.125</v>
+      </c>
+      <c r="R123">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="124" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>241</v>
+      </c>
+      <c r="B124">
+        <v>34</v>
+      </c>
+      <c r="C124" t="s">
+        <v>131</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="E124" t="s">
+        <v>450</v>
+      </c>
+      <c r="F124" t="s">
+        <v>167</v>
+      </c>
+      <c r="G124" t="s">
+        <v>146</v>
+      </c>
+      <c r="H124" t="s">
+        <v>146</v>
+      </c>
+      <c r="I124" s="1">
+        <v>45403</v>
+      </c>
+      <c r="J124" s="4">
+        <v>28.4809629890139</v>
+      </c>
+      <c r="K124" s="4">
+        <v>-81.467406691372901</v>
+      </c>
+      <c r="L124" s="6">
+        <v>50</v>
+      </c>
+      <c r="M124" t="s">
+        <v>50</v>
+      </c>
+      <c r="N124">
+        <v>1</v>
+      </c>
+      <c r="O124">
+        <v>15</v>
+      </c>
+      <c r="P124">
+        <f>2+5/16</f>
+        <v>2.3125</v>
+      </c>
+      <c r="Q124">
+        <f>2+2/16</f>
+        <v>2.125</v>
+      </c>
+      <c r="R124">
+        <f>1+14/16</f>
+        <v>1.875</v>
+      </c>
+    </row>
+    <row r="125" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>446</v>
+      </c>
+      <c r="B125">
+        <v>35</v>
+      </c>
+      <c r="C125" t="s">
+        <v>420</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="E125" t="s">
+        <v>450</v>
+      </c>
+      <c r="F125" t="s">
+        <v>167</v>
+      </c>
+      <c r="G125" t="s">
+        <v>146</v>
+      </c>
+      <c r="H125" t="s">
+        <v>146</v>
+      </c>
+      <c r="I125" s="1">
+        <v>45407</v>
+      </c>
+      <c r="J125" s="4">
+        <v>28.371808918683801</v>
+      </c>
+      <c r="K125" s="4">
+        <v>-81.517879136438097</v>
+      </c>
+      <c r="L125" s="6">
+        <v>51</v>
+      </c>
+      <c r="M125" t="s">
+        <v>50</v>
+      </c>
+      <c r="N125">
+        <v>1</v>
+      </c>
+      <c r="O125">
+        <v>14</v>
+      </c>
+      <c r="P125">
+        <f>2+2/16</f>
+        <v>2.125</v>
+      </c>
+      <c r="Q125">
+        <f>1+10/16</f>
+        <v>1.625</v>
+      </c>
+      <c r="R125">
+        <f>1+13/16</f>
+        <v>1.8125</v>
+      </c>
+    </row>
+    <row r="126" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>447</v>
+      </c>
+      <c r="B126">
+        <v>36</v>
+      </c>
+      <c r="C126" t="s">
+        <v>420</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="E126" t="s">
+        <v>452</v>
+      </c>
+      <c r="F126" t="s">
+        <v>167</v>
+      </c>
+      <c r="G126" t="s">
+        <v>146</v>
+      </c>
+      <c r="H126" t="s">
+        <v>146</v>
+      </c>
+      <c r="I126" s="1">
+        <v>45403</v>
+      </c>
+      <c r="J126" s="4">
+        <v>29.232650252891698</v>
+      </c>
+      <c r="K126" s="4">
+        <v>-81.107395234459503</v>
+      </c>
+      <c r="L126" s="6">
+        <v>52</v>
+      </c>
+      <c r="M126" t="s">
+        <v>449</v>
+      </c>
+      <c r="N126">
+        <v>1</v>
+      </c>
+      <c r="O126">
+        <v>48</v>
+      </c>
+      <c r="P126">
+        <v>3</v>
+      </c>
+      <c r="Q126">
+        <v>2.75</v>
+      </c>
+      <c r="R126">
+        <f>3+1/16</f>
+        <v>3.0625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed measurement data from in to cm
</commit_message>
<xml_diff>
--- a/data/duck_data.xlsx
+++ b/data/duck_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\Documents\DS_Projects\portfolio-deployments\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E6EEA9-2D26-4D15-B9BC-EDEDA8AA5788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C43914-BCB4-405D-9CD8-EDBD94FFB52A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15750" xr2:uid="{EF9DEEC2-186D-4161-AB80-57C24753F6AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EF9DEEC2-186D-4161-AB80-57C24753F6AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Ducks" sheetId="1" r:id="rId1"/>
@@ -1498,7 +1498,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1508,6 +1508,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1569,8 +1570,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55715085-9AFB-4516-817F-DC3F49C2B133}" name="Table1" displayName="Table1" ref="A1:R126" totalsRowShown="0">
   <autoFilter ref="A1:R126" xr:uid="{55715085-9AFB-4516-817F-DC3F49C2B133}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R98">
-    <sortCondition ref="I1:I98"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R126">
+    <sortCondition ref="I1:I126"/>
   </sortState>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{526AE2CE-1A5F-4A7A-B147-A0F5F581786F}" name="Duck"/>
@@ -1911,36 +1912,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B28BE0B7-C424-43DE-B13E-D21D7F7285C7}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:V126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="67" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L110" sqref="L110"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A39" sqref="A39"/>
+      <selection pane="topRight" activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="39.88671875" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="39.85546875" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1996,7 +2002,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -2053,7 +2059,7 @@
       </c>
       <c r="S2" s="2"/>
     </row>
-    <row r="3" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2110,7 +2116,7 @@
       </c>
       <c r="S3" s="2"/>
     </row>
-    <row r="4" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -2166,7 +2172,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -2223,7 +2229,7 @@
       </c>
       <c r="S5" s="2"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -2280,7 +2286,7 @@
       </c>
       <c r="S6" s="2"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -2336,7 +2342,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -2393,7 +2399,7 @@
       </c>
       <c r="V8" s="2"/>
     </row>
-    <row r="9" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -2450,7 +2456,7 @@
       </c>
       <c r="S9" s="2"/>
     </row>
-    <row r="10" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2503,7 +2509,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -2560,7 +2566,7 @@
       </c>
       <c r="S11" s="2"/>
     </row>
-    <row r="12" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -2617,7 +2623,7 @@
       </c>
       <c r="S12" s="2"/>
     </row>
-    <row r="13" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -2673,7 +2679,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -2730,7 +2736,7 @@
       </c>
       <c r="S14" s="2"/>
     </row>
-    <row r="15" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2787,7 +2793,7 @@
       </c>
       <c r="S15" s="2"/>
     </row>
-    <row r="16" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -2843,7 +2849,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -2900,7 +2906,7 @@
       </c>
       <c r="S17" s="2"/>
     </row>
-    <row r="18" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -2957,7 +2963,7 @@
       </c>
       <c r="S18" s="2"/>
     </row>
-    <row r="19" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -3013,7 +3019,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -3070,7 +3076,7 @@
       </c>
       <c r="S20" s="2"/>
     </row>
-    <row r="21" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -3127,7 +3133,7 @@
       </c>
       <c r="S21" s="2"/>
     </row>
-    <row r="22" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -3183,7 +3189,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -3240,7 +3246,7 @@
       </c>
       <c r="S23" s="2"/>
     </row>
-    <row r="24" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -3297,7 +3303,7 @@
       </c>
       <c r="S24" s="2"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -3353,7 +3359,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="144" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -3410,7 +3416,7 @@
       </c>
       <c r="S26" s="2"/>
     </row>
-    <row r="27" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -3467,7 +3473,7 @@
       </c>
       <c r="S27" s="2"/>
     </row>
-    <row r="28" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -3523,7 +3529,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -3580,7 +3586,7 @@
       </c>
       <c r="S29" s="2"/>
     </row>
-    <row r="30" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -3637,7 +3643,7 @@
       </c>
       <c r="S30" s="2"/>
     </row>
-    <row r="31" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>84</v>
       </c>
@@ -3693,7 +3699,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -3750,7 +3756,7 @@
       </c>
       <c r="S32" s="2"/>
     </row>
-    <row r="33" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>20</v>
       </c>
@@ -3807,7 +3813,7 @@
       </c>
       <c r="S33" s="2"/>
     </row>
-    <row r="34" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -3863,7 +3869,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -3922,7 +3928,7 @@
       </c>
       <c r="S35" s="2"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -3979,7 +3985,7 @@
       </c>
       <c r="S36" s="2"/>
     </row>
-    <row r="37" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -4035,7 +4041,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -4092,7 +4098,7 @@
       </c>
       <c r="S38" s="2"/>
     </row>
-    <row r="39" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>96</v>
       </c>
@@ -4149,7 +4155,7 @@
       </c>
       <c r="S39" s="2"/>
     </row>
-    <row r="40" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>97</v>
       </c>
@@ -4205,7 +4211,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>228</v>
       </c>
@@ -4261,7 +4267,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>229</v>
       </c>
@@ -4317,7 +4323,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>231</v>
       </c>
@@ -4373,7 +4379,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>232</v>
       </c>
@@ -4429,7 +4435,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>241</v>
       </c>
@@ -4485,7 +4491,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>242</v>
       </c>
@@ -4541,7 +4547,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>243</v>
       </c>
@@ -4597,7 +4603,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>244</v>
       </c>
@@ -4653,7 +4659,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>331</v>
       </c>
@@ -4699,19 +4705,17 @@
       <c r="O49">
         <v>50</v>
       </c>
-      <c r="P49">
-        <f>2+15/16</f>
-        <v>2.9375</v>
-      </c>
-      <c r="Q49">
-        <v>3.75</v>
-      </c>
-      <c r="R49">
-        <f>3+13/16</f>
-        <v>3.8125</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="P49" s="7">
+        <v>7.5</v>
+      </c>
+      <c r="Q49" s="7">
+        <v>9.5</v>
+      </c>
+      <c r="R49" s="7">
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>332</v>
       </c>
@@ -4757,18 +4761,17 @@
       <c r="O50">
         <v>47</v>
       </c>
-      <c r="P50">
-        <v>3</v>
-      </c>
-      <c r="Q50">
-        <f>3+14/16</f>
-        <v>3.875</v>
-      </c>
-      <c r="R50">
-        <v>3.125</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P50" s="7">
+        <v>7.6</v>
+      </c>
+      <c r="Q50" s="7">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="R50" s="7">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>333</v>
       </c>
@@ -4814,20 +4817,17 @@
       <c r="O51">
         <v>36</v>
       </c>
-      <c r="P51">
-        <f>2+13/16</f>
-        <v>2.8125</v>
-      </c>
-      <c r="Q51">
-        <f>2+6/16</f>
-        <v>2.375</v>
-      </c>
-      <c r="R51">
-        <f>3+1/16</f>
-        <v>3.0625</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="P51" s="7">
+        <v>7.1</v>
+      </c>
+      <c r="Q51" s="7">
+        <v>6</v>
+      </c>
+      <c r="R51" s="7">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>272</v>
       </c>
@@ -4873,17 +4873,17 @@
       <c r="O52">
         <v>17</v>
       </c>
-      <c r="P52">
+      <c r="P52" s="7">
         <v>5.4</v>
       </c>
-      <c r="Q52">
+      <c r="Q52" s="7">
         <v>4.5</v>
       </c>
-      <c r="R52">
+      <c r="R52" s="7">
         <v>4.7</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>245</v>
       </c>
@@ -4929,17 +4929,17 @@
       <c r="O53">
         <v>17</v>
       </c>
-      <c r="P53">
+      <c r="P53" s="7">
         <v>5.4</v>
       </c>
-      <c r="Q53">
+      <c r="Q53" s="7">
         <v>5.6</v>
       </c>
-      <c r="R53">
+      <c r="R53" s="7">
         <v>5.8</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>246</v>
       </c>
@@ -4985,17 +4985,17 @@
       <c r="O54">
         <v>18</v>
       </c>
-      <c r="P54">
+      <c r="P54" s="7">
         <v>6.1</v>
       </c>
-      <c r="Q54">
+      <c r="Q54" s="7">
         <v>5.7</v>
       </c>
-      <c r="R54">
+      <c r="R54" s="7">
         <v>5.9</v>
       </c>
     </row>
-    <row r="55" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>247</v>
       </c>
@@ -5041,17 +5041,17 @@
       <c r="O55">
         <v>17</v>
       </c>
-      <c r="P55">
+      <c r="P55" s="7">
         <v>5.7</v>
       </c>
-      <c r="Q55">
+      <c r="Q55" s="7">
         <v>5.7</v>
       </c>
-      <c r="R55">
+      <c r="R55" s="7">
         <v>5.8</v>
       </c>
     </row>
-    <row r="56" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>248</v>
       </c>
@@ -5097,17 +5097,17 @@
       <c r="O56">
         <v>19</v>
       </c>
-      <c r="P56">
+      <c r="P56" s="7">
         <v>5.8</v>
       </c>
-      <c r="Q56">
+      <c r="Q56" s="7">
         <v>5.7</v>
       </c>
-      <c r="R56">
+      <c r="R56" s="7">
         <v>5.9</v>
       </c>
     </row>
-    <row r="57" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>257</v>
       </c>
@@ -5153,17 +5153,17 @@
       <c r="O57">
         <v>155</v>
       </c>
-      <c r="P57">
+      <c r="P57" s="7">
         <v>11.5</v>
       </c>
-      <c r="Q57">
+      <c r="Q57" s="7">
         <v>8.1</v>
       </c>
-      <c r="R57">
+      <c r="R57" s="7">
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>258</v>
       </c>
@@ -5209,17 +5209,17 @@
       <c r="O58">
         <v>9</v>
       </c>
-      <c r="P58">
+      <c r="P58" s="7">
         <v>3.3</v>
       </c>
-      <c r="Q58">
+      <c r="Q58" s="7">
         <v>4.7</v>
       </c>
-      <c r="R58">
+      <c r="R58" s="7">
         <v>5.4</v>
       </c>
     </row>
-    <row r="59" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>259</v>
       </c>
@@ -5265,17 +5265,17 @@
       <c r="O59">
         <v>11</v>
       </c>
-      <c r="P59">
+      <c r="P59" s="7">
         <v>6.4</v>
       </c>
-      <c r="Q59">
+      <c r="Q59" s="7">
         <v>3.3</v>
       </c>
-      <c r="R59">
+      <c r="R59" s="7">
         <v>4.3</v>
       </c>
     </row>
-    <row r="60" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>275</v>
       </c>
@@ -5321,18 +5321,17 @@
       <c r="O60">
         <v>145</v>
       </c>
-      <c r="P60">
-        <f>2+14/16</f>
-        <v>2.875</v>
-      </c>
-      <c r="Q60">
-        <v>2.5</v>
-      </c>
-      <c r="R60">
-        <v>3.25</v>
-      </c>
-    </row>
-    <row r="61" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="P60" s="7">
+        <v>7.3</v>
+      </c>
+      <c r="Q60" s="7">
+        <v>6.4</v>
+      </c>
+      <c r="R60" s="7">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>273</v>
       </c>
@@ -5378,19 +5377,17 @@
       <c r="O61">
         <v>107</v>
       </c>
-      <c r="P61">
-        <f>3+13/16</f>
-        <v>3.8125</v>
-      </c>
-      <c r="Q61">
-        <v>3.25</v>
-      </c>
-      <c r="R61">
-        <f>4+10/16</f>
-        <v>4.625</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="P61" s="7">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="Q61" s="7">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="R61" s="7">
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>274</v>
       </c>
@@ -5436,17 +5433,17 @@
       <c r="O62">
         <v>102</v>
       </c>
-      <c r="P62">
-        <v>3.75</v>
-      </c>
-      <c r="Q62">
-        <v>3.5</v>
-      </c>
-      <c r="R62">
-        <v>4.75</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P62" s="7">
+        <v>9.5</v>
+      </c>
+      <c r="Q62" s="7">
+        <v>8.9</v>
+      </c>
+      <c r="R62" s="7">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>314</v>
       </c>
@@ -5492,19 +5489,17 @@
       <c r="O63">
         <v>86</v>
       </c>
-      <c r="P63">
-        <f>3+4/16</f>
-        <v>3.25</v>
-      </c>
-      <c r="Q63">
-        <v>2.75</v>
-      </c>
-      <c r="R63">
-        <f>3+9/16</f>
-        <v>3.5625</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P63" s="7">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="Q63" s="7">
+        <v>7</v>
+      </c>
+      <c r="R63" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>281</v>
       </c>
@@ -5550,18 +5545,17 @@
       <c r="O64">
         <v>18</v>
       </c>
-      <c r="P64">
-        <v>2</v>
-      </c>
-      <c r="Q64">
-        <v>2.125</v>
-      </c>
-      <c r="R64">
-        <f>2+7/16</f>
-        <v>2.4375</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P64" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="Q64" s="7">
+        <v>5.4</v>
+      </c>
+      <c r="R64" s="7">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>289</v>
       </c>
@@ -5607,19 +5601,17 @@
       <c r="O65">
         <v>21</v>
       </c>
-      <c r="P65">
-        <f>2+3/16</f>
-        <v>2.1875</v>
-      </c>
-      <c r="Q65">
-        <f>2+5/16</f>
-        <v>2.3125</v>
-      </c>
-      <c r="R65">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="P65" s="7">
+        <v>5.6</v>
+      </c>
+      <c r="Q65" s="7">
+        <v>5.9</v>
+      </c>
+      <c r="R65" s="7">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>290</v>
       </c>
@@ -5665,18 +5657,17 @@
       <c r="O66">
         <v>24</v>
       </c>
-      <c r="P66">
-        <f>2+9/16</f>
-        <v>2.5625</v>
-      </c>
-      <c r="Q66">
-        <v>2</v>
-      </c>
-      <c r="R66">
-        <v>2.25</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P66" s="7">
+        <v>6.5</v>
+      </c>
+      <c r="Q66" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="R66" s="7">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>291</v>
       </c>
@@ -5722,18 +5713,17 @@
       <c r="O67">
         <v>26</v>
       </c>
-      <c r="P67">
-        <v>2.625</v>
-      </c>
-      <c r="Q67">
-        <v>2.25</v>
-      </c>
-      <c r="R67">
-        <f>2+3/16</f>
-        <v>2.1875</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P67" s="7">
+        <v>6.7</v>
+      </c>
+      <c r="Q67" s="7">
+        <v>5.7</v>
+      </c>
+      <c r="R67" s="7">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>305</v>
       </c>
@@ -5779,18 +5769,17 @@
       <c r="O68">
         <v>162</v>
       </c>
-      <c r="P68">
-        <v>5.25</v>
-      </c>
-      <c r="Q68">
-        <f>5+6/16</f>
-        <v>5.375</v>
-      </c>
-      <c r="R68">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P68" s="7">
+        <v>13.3</v>
+      </c>
+      <c r="Q68" s="7">
+        <v>13.7</v>
+      </c>
+      <c r="R68" s="7">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>307</v>
       </c>
@@ -5836,18 +5825,17 @@
       <c r="O69">
         <v>25</v>
       </c>
-      <c r="P69">
-        <f>2+15/16</f>
-        <v>2.9375</v>
-      </c>
-      <c r="Q69">
-        <v>2.125</v>
-      </c>
-      <c r="R69">
-        <v>2.125</v>
-      </c>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P69" s="7">
+        <v>7.5</v>
+      </c>
+      <c r="Q69" s="7">
+        <v>5.4</v>
+      </c>
+      <c r="R69" s="7">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>308</v>
       </c>
@@ -5893,20 +5881,17 @@
       <c r="O70">
         <v>24</v>
       </c>
-      <c r="P70">
-        <f>2+10/16</f>
-        <v>2.625</v>
-      </c>
-      <c r="Q70">
-        <f>1+15/16</f>
-        <v>1.9375</v>
-      </c>
-      <c r="R70">
-        <f>2+13/16</f>
-        <v>2.8125</v>
-      </c>
-    </row>
-    <row r="71" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="P70" s="7">
+        <v>6.7</v>
+      </c>
+      <c r="Q70" s="7">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="R70" s="7">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>280</v>
       </c>
@@ -5952,17 +5937,17 @@
       <c r="O71">
         <v>39</v>
       </c>
-      <c r="P71">
-        <v>2.5</v>
-      </c>
-      <c r="Q71">
-        <v>2.5</v>
-      </c>
-      <c r="R71">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P71" s="7">
+        <v>6.4</v>
+      </c>
+      <c r="Q71" s="7">
+        <v>6.4</v>
+      </c>
+      <c r="R71" s="7">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>279</v>
       </c>
@@ -6008,17 +5993,17 @@
       <c r="O72">
         <v>163</v>
       </c>
-      <c r="P72">
-        <v>2.48</v>
-      </c>
-      <c r="Q72">
-        <v>2.4</v>
-      </c>
-      <c r="R72">
-        <v>2.69</v>
-      </c>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P72" s="7">
+        <v>6.3</v>
+      </c>
+      <c r="Q72" s="7">
+        <v>6.1</v>
+      </c>
+      <c r="R72" s="7">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>282</v>
       </c>
@@ -6064,18 +6049,17 @@
       <c r="O73">
         <v>56</v>
       </c>
-      <c r="P73">
-        <v>3.25</v>
-      </c>
-      <c r="Q73">
-        <f>3+2/16</f>
-        <v>3.125</v>
-      </c>
-      <c r="R73">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P73" s="7">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="Q73" s="7">
+        <v>7.9</v>
+      </c>
+      <c r="R73" s="7">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>285</v>
       </c>
@@ -6121,18 +6105,17 @@
       <c r="O74">
         <v>56</v>
       </c>
-      <c r="P74">
-        <v>3.25</v>
-      </c>
-      <c r="Q74">
-        <f>3+5/16</f>
-        <v>3.3125</v>
-      </c>
-      <c r="R74">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P74" s="7">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="Q74" s="7">
+        <v>8.4</v>
+      </c>
+      <c r="R74" s="7">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>286</v>
       </c>
@@ -6178,18 +6161,17 @@
       <c r="O75">
         <v>55</v>
       </c>
-      <c r="P75">
-        <f>3+6/16</f>
-        <v>3.375</v>
-      </c>
-      <c r="Q75">
-        <v>3.125</v>
-      </c>
-      <c r="R75">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P75" s="7">
+        <v>8.6</v>
+      </c>
+      <c r="Q75" s="7">
+        <v>7.9</v>
+      </c>
+      <c r="R75" s="7">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>287</v>
       </c>
@@ -6235,19 +6217,17 @@
       <c r="O76">
         <v>55</v>
       </c>
-      <c r="P76">
-        <f>3+5/16</f>
-        <v>3.3125</v>
-      </c>
-      <c r="Q76">
-        <f>3+13/16</f>
-        <v>3.8125</v>
-      </c>
-      <c r="R76">
-        <v>3.625</v>
-      </c>
-    </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P76" s="7">
+        <v>8.4</v>
+      </c>
+      <c r="Q76" s="7">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="R76" s="7">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>283</v>
       </c>
@@ -6293,18 +6273,17 @@
       <c r="O77">
         <v>62</v>
       </c>
-      <c r="P77">
-        <v>3.125</v>
-      </c>
-      <c r="Q77">
-        <f>3+14/16</f>
-        <v>3.875</v>
-      </c>
-      <c r="R77">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P77" s="7">
+        <v>7.9</v>
+      </c>
+      <c r="Q77" s="7">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="R77" s="7">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>284</v>
       </c>
@@ -6350,17 +6329,17 @@
       <c r="O78">
         <v>116</v>
       </c>
-      <c r="P78">
-        <v>3.125</v>
-      </c>
-      <c r="Q78">
-        <v>2.625</v>
-      </c>
-      <c r="R78">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P78" s="7">
+        <v>7.9</v>
+      </c>
+      <c r="Q78" s="7">
+        <v>6.7</v>
+      </c>
+      <c r="R78" s="7">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>288</v>
       </c>
@@ -6406,20 +6385,17 @@
       <c r="O79">
         <v>67</v>
       </c>
-      <c r="P79">
-        <f>4+7/16</f>
-        <v>4.4375</v>
-      </c>
-      <c r="Q79">
-        <f>3+1/16</f>
-        <v>3.0625</v>
-      </c>
-      <c r="R79">
-        <f>4+1/16</f>
-        <v>4.0625</v>
-      </c>
-    </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P79" s="7">
+        <v>11.3</v>
+      </c>
+      <c r="Q79" s="7">
+        <v>7.8</v>
+      </c>
+      <c r="R79" s="7">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>306</v>
       </c>
@@ -6465,20 +6441,17 @@
       <c r="O80">
         <v>59</v>
       </c>
-      <c r="P80">
-        <f>3+13/16</f>
-        <v>3.8125</v>
-      </c>
-      <c r="Q80">
-        <f>3+14/16</f>
-        <v>3.875</v>
-      </c>
-      <c r="R80">
-        <f>3+7/16</f>
-        <v>3.4375</v>
-      </c>
-    </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P80" s="7">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="Q80" s="7">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="R80" s="7">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>309</v>
       </c>
@@ -6524,19 +6497,17 @@
       <c r="O81">
         <v>54</v>
       </c>
-      <c r="P81">
-        <v>3.125</v>
-      </c>
-      <c r="Q81">
-        <f>3+7/16</f>
-        <v>3.4375</v>
-      </c>
-      <c r="R81">
-        <f>4+13/16</f>
-        <v>4.8125</v>
-      </c>
-    </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P81" s="7">
+        <v>7.9</v>
+      </c>
+      <c r="Q81" s="7">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="R81" s="7">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>310</v>
       </c>
@@ -6582,19 +6553,17 @@
       <c r="O82">
         <v>95</v>
       </c>
-      <c r="P82">
-        <f>3+1/16</f>
-        <v>3.0625</v>
-      </c>
-      <c r="Q82">
-        <v>4.875</v>
-      </c>
-      <c r="R82">
-        <f>4+14/16</f>
-        <v>4.875</v>
-      </c>
-    </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P82" s="7">
+        <v>7.8</v>
+      </c>
+      <c r="Q82" s="7">
+        <v>12.4</v>
+      </c>
+      <c r="R82" s="7">
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>311</v>
       </c>
@@ -6640,20 +6609,17 @@
       <c r="O83">
         <v>0.1</v>
       </c>
-      <c r="P83">
-        <f>10/16</f>
-        <v>0.625</v>
-      </c>
-      <c r="Q83">
-        <f>9/16</f>
-        <v>0.5625</v>
-      </c>
-      <c r="R83">
-        <f>9/16</f>
-        <v>0.5625</v>
-      </c>
-    </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P83" s="7">
+        <v>1.6</v>
+      </c>
+      <c r="Q83" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="R83" s="7">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>303</v>
       </c>
@@ -6699,19 +6665,17 @@
       <c r="O84">
         <v>42</v>
       </c>
-      <c r="P84">
-        <f>3+14/16</f>
-        <v>3.875</v>
-      </c>
-      <c r="Q84">
-        <f>3+11/16</f>
-        <v>3.6875</v>
-      </c>
-      <c r="R84">
-        <v>3.25</v>
-      </c>
-    </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P84" s="7">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="Q84" s="7">
+        <v>9.4</v>
+      </c>
+      <c r="R84" s="7">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>304</v>
       </c>
@@ -6757,18 +6721,17 @@
       <c r="O85">
         <v>48</v>
       </c>
-      <c r="P85">
-        <f>3+5/16</f>
-        <v>3.3125</v>
-      </c>
-      <c r="Q85">
-        <v>3.75</v>
-      </c>
-      <c r="R85">
-        <v>3.625</v>
-      </c>
-    </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P85" s="7">
+        <v>8.4</v>
+      </c>
+      <c r="Q85" s="7">
+        <v>9.5</v>
+      </c>
+      <c r="R85" s="7">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>317</v>
       </c>
@@ -6814,17 +6777,17 @@
       <c r="O86">
         <v>66</v>
       </c>
-      <c r="P86">
-        <v>2.8125</v>
-      </c>
-      <c r="Q86">
-        <v>2.875</v>
-      </c>
-      <c r="R86">
-        <v>3.3125</v>
-      </c>
-    </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P86" s="7">
+        <v>7.1</v>
+      </c>
+      <c r="Q86" s="7">
+        <v>7.3</v>
+      </c>
+      <c r="R86" s="7">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>318</v>
       </c>
@@ -6870,19 +6833,17 @@
       <c r="O87">
         <v>22</v>
       </c>
-      <c r="P87">
-        <f>2+11/16</f>
-        <v>2.6875</v>
-      </c>
-      <c r="Q87">
-        <v>2</v>
-      </c>
-      <c r="R87">
-        <f>2+3/16</f>
-        <v>2.1875</v>
-      </c>
-    </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P87" s="7">
+        <v>6.8</v>
+      </c>
+      <c r="Q87" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="R87" s="7">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>320</v>
       </c>
@@ -6928,19 +6889,17 @@
       <c r="O88">
         <v>17</v>
       </c>
-      <c r="P88">
-        <f>1+9/16</f>
-        <v>1.5625</v>
-      </c>
-      <c r="Q88">
-        <v>1.75</v>
-      </c>
-      <c r="R88">
-        <f>1+13/16</f>
-        <v>1.8125</v>
-      </c>
-    </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P88" s="7">
+        <v>4</v>
+      </c>
+      <c r="Q88" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="R88" s="7">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>322</v>
       </c>
@@ -6986,20 +6945,17 @@
       <c r="O89">
         <v>19</v>
       </c>
-      <c r="P89">
-        <f>2+6/16</f>
-        <v>2.375</v>
-      </c>
-      <c r="Q89">
-        <f>1+7/8</f>
-        <v>1.875</v>
-      </c>
-      <c r="R89">
-        <f>2+7/16</f>
-        <v>2.4375</v>
-      </c>
-    </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P89" s="7">
+        <v>6</v>
+      </c>
+      <c r="Q89" s="7">
+        <v>4.8</v>
+      </c>
+      <c r="R89" s="7">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>321</v>
       </c>
@@ -7045,17 +7001,17 @@
       <c r="O90">
         <v>15</v>
       </c>
-      <c r="P90">
-        <v>2.875</v>
-      </c>
-      <c r="Q90">
-        <v>2</v>
-      </c>
-      <c r="R90">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P90" s="7">
+        <v>7.3</v>
+      </c>
+      <c r="Q90" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="R90" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>323</v>
       </c>
@@ -7101,19 +7057,17 @@
       <c r="O91">
         <v>18</v>
       </c>
-      <c r="P91">
-        <f>2+7/16</f>
-        <v>2.4375</v>
-      </c>
-      <c r="Q91">
-        <v>1.9375</v>
-      </c>
-      <c r="R91">
-        <f>1.375</f>
-        <v>1.375</v>
-      </c>
-    </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P91" s="7">
+        <v>6.2</v>
+      </c>
+      <c r="Q91" s="7">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="R91" s="7">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>324</v>
       </c>
@@ -7159,19 +7113,17 @@
       <c r="O92">
         <v>17</v>
       </c>
-      <c r="P92">
-        <f>1+15/16</f>
-        <v>1.9375</v>
-      </c>
-      <c r="Q92">
-        <f>1+7/8</f>
-        <v>1.875</v>
-      </c>
-      <c r="R92">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P92" s="7">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="Q92" s="7">
+        <v>4.8</v>
+      </c>
+      <c r="R92" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>325</v>
       </c>
@@ -7217,18 +7169,17 @@
       <c r="O93">
         <v>14</v>
       </c>
-      <c r="P93">
-        <v>1.9375</v>
-      </c>
-      <c r="Q93">
-        <f>1+13/16</f>
-        <v>1.8125</v>
-      </c>
-      <c r="R93">
-        <v>1.875</v>
-      </c>
-    </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P93" s="7">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="Q93" s="7">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="R93" s="7">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>341</v>
       </c>
@@ -7274,19 +7225,17 @@
       <c r="O94">
         <v>6</v>
       </c>
-      <c r="P94">
-        <v>1.125</v>
-      </c>
-      <c r="Q94">
-        <f>1+7/16</f>
-        <v>1.4375</v>
-      </c>
-      <c r="R94">
-        <f>1+5/16</f>
-        <v>1.3125</v>
-      </c>
-    </row>
-    <row r="95" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="P94" s="7">
+        <v>2.9</v>
+      </c>
+      <c r="Q94" s="7">
+        <v>3.7</v>
+      </c>
+      <c r="R94" s="7">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>340</v>
       </c>
@@ -7332,19 +7281,17 @@
       <c r="O95">
         <v>43</v>
       </c>
-      <c r="P95">
-        <v>3</v>
-      </c>
-      <c r="Q95">
-        <f>2+14/16</f>
-        <v>2.875</v>
-      </c>
-      <c r="R95">
-        <f>3+5/16</f>
-        <v>3.3125</v>
-      </c>
-    </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P95" s="7">
+        <v>7.6</v>
+      </c>
+      <c r="Q95" s="7">
+        <v>7.3</v>
+      </c>
+      <c r="R95" s="7">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>338</v>
       </c>
@@ -7390,18 +7337,17 @@
       <c r="O96">
         <v>45</v>
       </c>
-      <c r="P96">
-        <f>3+5/16</f>
-        <v>3.3125</v>
-      </c>
-      <c r="Q96">
-        <v>3.875</v>
-      </c>
-      <c r="R96">
-        <v>3.125</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P96" s="7">
+        <v>8.4</v>
+      </c>
+      <c r="Q96" s="7">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="R96" s="7">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>347</v>
       </c>
@@ -7447,18 +7393,17 @@
       <c r="O97">
         <v>48</v>
       </c>
-      <c r="P97">
-        <f>3+6/16</f>
-        <v>3.375</v>
-      </c>
-      <c r="Q97">
-        <v>3.875</v>
-      </c>
-      <c r="R97">
-        <v>3.125</v>
-      </c>
-    </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P97" s="7">
+        <v>8.6</v>
+      </c>
+      <c r="Q97" s="7">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="R97" s="7">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>339</v>
       </c>
@@ -7504,18 +7449,17 @@
       <c r="O98">
         <v>47</v>
       </c>
-      <c r="P98">
-        <f>3+6/16</f>
-        <v>3.375</v>
-      </c>
-      <c r="Q98">
-        <v>3.875</v>
-      </c>
-      <c r="R98">
-        <v>3.125</v>
-      </c>
-    </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P98" s="7">
+        <v>8.6</v>
+      </c>
+      <c r="Q98" s="7">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="R98" s="7">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>395</v>
       </c>
@@ -7561,17 +7505,17 @@
       <c r="O99">
         <v>153</v>
       </c>
-      <c r="P99">
-        <v>5</v>
-      </c>
-      <c r="Q99">
-        <v>5.25</v>
-      </c>
-      <c r="R99">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P99" s="7">
+        <v>12.7</v>
+      </c>
+      <c r="Q99" s="7">
+        <v>13.3</v>
+      </c>
+      <c r="R99" s="7">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>396</v>
       </c>
@@ -7617,20 +7561,17 @@
       <c r="O100">
         <v>19</v>
       </c>
-      <c r="P100">
-        <f>1+15/16</f>
-        <v>1.9375</v>
-      </c>
-      <c r="Q100">
-        <f>1+14/16</f>
-        <v>1.875</v>
-      </c>
-      <c r="R100">
-        <f>2+5/16</f>
-        <v>2.3125</v>
-      </c>
-    </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P100" s="7">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="Q100" s="7">
+        <v>4.8</v>
+      </c>
+      <c r="R100" s="7">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>397</v>
       </c>
@@ -7676,19 +7617,17 @@
       <c r="O101">
         <v>19</v>
       </c>
-      <c r="P101">
-        <v>2</v>
-      </c>
-      <c r="Q101">
-        <f>1+14/16</f>
-        <v>1.875</v>
-      </c>
-      <c r="R101">
-        <f>2+5/16</f>
-        <v>2.3125</v>
-      </c>
-    </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P101" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="Q101" s="7">
+        <v>4.8</v>
+      </c>
+      <c r="R101" s="7">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>398</v>
       </c>
@@ -7734,19 +7673,17 @@
       <c r="O102">
         <v>18</v>
       </c>
-      <c r="P102">
-        <v>2</v>
-      </c>
-      <c r="Q102">
-        <f>1+14/16</f>
-        <v>1.875</v>
-      </c>
-      <c r="R102">
-        <f>2+3/16</f>
-        <v>2.1875</v>
-      </c>
-    </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P102" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="Q102" s="7">
+        <v>4.8</v>
+      </c>
+      <c r="R102" s="7">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>399</v>
       </c>
@@ -7792,20 +7729,17 @@
       <c r="O103">
         <v>18</v>
       </c>
-      <c r="P103">
-        <f>2+1/16</f>
-        <v>2.0625</v>
-      </c>
-      <c r="Q103">
-        <f>1+14/16</f>
-        <v>1.875</v>
-      </c>
-      <c r="R103">
-        <f>2+2/16</f>
-        <v>2.125</v>
-      </c>
-    </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P103" s="7">
+        <v>5.2</v>
+      </c>
+      <c r="Q103" s="7">
+        <v>4.8</v>
+      </c>
+      <c r="R103" s="7">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>400</v>
       </c>
@@ -7851,19 +7785,17 @@
       <c r="O104">
         <v>22</v>
       </c>
-      <c r="P104">
-        <v>2.5</v>
-      </c>
-      <c r="Q104">
-        <f>1+15/16</f>
-        <v>1.9375</v>
-      </c>
-      <c r="R104">
-        <f>2+2/16</f>
-        <v>2.125</v>
-      </c>
-    </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P104" s="7">
+        <v>6.4</v>
+      </c>
+      <c r="Q104" s="7">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="R104" s="7">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>410</v>
       </c>
@@ -7909,20 +7841,17 @@
       <c r="O105">
         <v>20</v>
       </c>
-      <c r="P105">
-        <f>2+5/16</f>
-        <v>2.3125</v>
-      </c>
-      <c r="Q105">
-        <f>1+11/16</f>
-        <v>1.6875</v>
-      </c>
-      <c r="R105">
-        <f>2+7/16</f>
-        <v>2.4375</v>
-      </c>
-    </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P105" s="7">
+        <v>5.9</v>
+      </c>
+      <c r="Q105" s="7">
+        <v>4.3</v>
+      </c>
+      <c r="R105" s="7">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>409</v>
       </c>
@@ -7968,18 +7897,17 @@
       <c r="O106">
         <v>70</v>
       </c>
-      <c r="P106">
-        <f>2.625</f>
-        <v>2.625</v>
-      </c>
-      <c r="Q106">
-        <v>3</v>
-      </c>
-      <c r="R106">
-        <v>2.625</v>
-      </c>
-    </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P106" s="7">
+        <v>6.7</v>
+      </c>
+      <c r="Q106" s="7">
+        <v>7.6</v>
+      </c>
+      <c r="R106" s="7">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>412</v>
       </c>
@@ -8025,19 +7953,17 @@
       <c r="O107">
         <v>17</v>
       </c>
-      <c r="P107">
-        <v>2.25</v>
-      </c>
-      <c r="Q107">
-        <f>1+14/16</f>
-        <v>1.875</v>
-      </c>
-      <c r="R107">
-        <f>1+14/16</f>
-        <v>1.875</v>
-      </c>
-    </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P107" s="7">
+        <v>5.7</v>
+      </c>
+      <c r="Q107" s="7">
+        <v>4.8</v>
+      </c>
+      <c r="R107" s="7">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>411</v>
       </c>
@@ -8083,18 +8009,17 @@
       <c r="O108">
         <v>15</v>
       </c>
-      <c r="P108">
-        <v>2</v>
-      </c>
-      <c r="Q108">
-        <f>1+13/16</f>
-        <v>1.8125</v>
-      </c>
-      <c r="R108">
-        <v>1.875</v>
-      </c>
-    </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P108" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="Q108" s="7">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="R108" s="7">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>413</v>
       </c>
@@ -8140,17 +8065,17 @@
       <c r="O109">
         <v>54</v>
       </c>
-      <c r="P109">
-        <v>3</v>
-      </c>
-      <c r="Q109">
-        <v>2.625</v>
-      </c>
-      <c r="R109">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P109" s="7">
+        <v>7.6</v>
+      </c>
+      <c r="Q109" s="7">
+        <v>6.7</v>
+      </c>
+      <c r="R109" s="7">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>421</v>
       </c>
@@ -8196,18 +8121,17 @@
       <c r="O110">
         <v>17</v>
       </c>
-      <c r="P110">
-        <v>1.75</v>
-      </c>
-      <c r="Q110">
-        <f>1+13/16</f>
-        <v>1.8125</v>
-      </c>
-      <c r="R110">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P110" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Q110" s="7">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="R110" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>422</v>
       </c>
@@ -8253,36 +8177,34 @@
       <c r="O111">
         <v>68</v>
       </c>
-      <c r="P111">
-        <v>3.5</v>
-      </c>
-      <c r="Q111">
-        <f>3+6/16</f>
-        <v>3.375</v>
-      </c>
-      <c r="R111">
-        <f>3+9/16</f>
-        <v>3.5625</v>
-      </c>
-    </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P111" s="7">
+        <v>8.9</v>
+      </c>
+      <c r="Q111" s="7">
+        <v>8.6</v>
+      </c>
+      <c r="R111" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>425</v>
+        <v>432</v>
       </c>
       <c r="B112">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C112" t="s">
         <v>420</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="E112" t="s">
-        <v>133</v>
+        <v>440</v>
       </c>
       <c r="F112" t="s">
-        <v>26</v>
+        <v>165</v>
       </c>
       <c r="G112" t="s">
         <v>146</v>
@@ -8291,13 +8213,13 @@
         <v>146</v>
       </c>
       <c r="I112" s="1">
-        <v>45346</v>
+        <v>45270</v>
       </c>
       <c r="J112" s="4">
-        <v>38.892167999999998</v>
+        <v>42.787076999999996</v>
       </c>
       <c r="K112" s="4">
-        <v>-77.025794000000005</v>
+        <v>-71.503960000000006</v>
       </c>
       <c r="L112" s="6">
         <v>46</v>
@@ -8306,40 +8228,39 @@
         <v>50</v>
       </c>
       <c r="N112">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O112">
-        <v>65</v>
-      </c>
-      <c r="P112">
+        <v>8</v>
+      </c>
+      <c r="P112" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="Q112" s="7">
+        <v>3.7</v>
+      </c>
+      <c r="R112" s="7">
         <v>3.5</v>
       </c>
-      <c r="Q112">
-        <f>3+3/16</f>
-        <v>3.1875</v>
-      </c>
-      <c r="R112">
-        <v>4.1875</v>
-      </c>
-    </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="B113">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C113" t="s">
         <v>420</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>433</v>
+        <v>230</v>
       </c>
       <c r="E113" t="s">
-        <v>133</v>
+        <v>327</v>
       </c>
       <c r="F113" t="s">
-        <v>26</v>
+        <v>163</v>
       </c>
       <c r="G113" t="s">
         <v>146</v>
@@ -8348,13 +8269,13 @@
         <v>146</v>
       </c>
       <c r="I113" s="1">
-        <v>45346</v>
+        <v>45311</v>
       </c>
       <c r="J113" s="4">
-        <v>38.892167999999998</v>
+        <v>39.056086162518199</v>
       </c>
       <c r="K113" s="4">
-        <v>-77.025794000000005</v>
+        <v>-77.114897400000004</v>
       </c>
       <c r="L113" s="6">
         <v>46</v>
@@ -8366,37 +8287,36 @@
         <v>1</v>
       </c>
       <c r="O113">
-        <v>64</v>
-      </c>
-      <c r="P113">
-        <v>3.25</v>
-      </c>
-      <c r="Q113">
-        <v>3.1875</v>
-      </c>
-      <c r="R113">
-        <f>4+14/16</f>
-        <v>4.875</v>
-      </c>
-    </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="P113" s="7">
+        <v>6.4</v>
+      </c>
+      <c r="Q113" s="7">
+        <v>6</v>
+      </c>
+      <c r="R113" s="7">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="B114">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C114" t="s">
         <v>420</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>434</v>
+        <v>230</v>
       </c>
       <c r="E114" t="s">
-        <v>437</v>
+        <v>327</v>
       </c>
       <c r="F114" t="s">
-        <v>438</v>
+        <v>163</v>
       </c>
       <c r="G114" t="s">
         <v>146</v>
@@ -8405,13 +8325,13 @@
         <v>146</v>
       </c>
       <c r="I114" s="1">
-        <v>45355</v>
+        <v>45311</v>
       </c>
       <c r="J114" s="4">
-        <v>33.246605000000002</v>
+        <v>39.056086162518199</v>
       </c>
       <c r="K114" s="4">
-        <v>-111.84272</v>
+        <v>-77.114897400000004</v>
       </c>
       <c r="L114" s="6">
         <v>46</v>
@@ -8423,38 +8343,36 @@
         <v>1</v>
       </c>
       <c r="O114">
-        <v>18</v>
-      </c>
-      <c r="P114">
-        <f>2+13/16</f>
-        <v>2.8125</v>
-      </c>
-      <c r="Q114">
-        <v>2</v>
-      </c>
-      <c r="R114">
-        <f>2+1/16</f>
-        <v>2.0625</v>
-      </c>
-    </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="P114" s="7">
+        <v>7</v>
+      </c>
+      <c r="Q114" s="7">
+        <v>6</v>
+      </c>
+      <c r="R114" s="7">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B115">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C115" t="s">
         <v>420</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E115" t="s">
-        <v>436</v>
+        <v>133</v>
       </c>
       <c r="F115" t="s">
-        <v>439</v>
+        <v>26</v>
       </c>
       <c r="G115" t="s">
         <v>146</v>
@@ -8463,13 +8381,13 @@
         <v>146</v>
       </c>
       <c r="I115" s="1">
-        <v>45353</v>
+        <v>45346</v>
       </c>
       <c r="J115" s="4">
-        <v>33.980536999999998</v>
+        <v>38.892167999999998</v>
       </c>
       <c r="K115" s="4">
-        <v>-84.424716000000004</v>
+        <v>-77.025794000000005</v>
       </c>
       <c r="L115" s="6">
         <v>46</v>
@@ -8481,37 +8399,37 @@
         <v>1</v>
       </c>
       <c r="O115">
-        <v>16</v>
-      </c>
-      <c r="P115">
-        <v>2</v>
-      </c>
-      <c r="Q115">
-        <v>2.875</v>
-      </c>
-      <c r="R115">
-        <v>2.0625</v>
-      </c>
-    </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="P115" s="7">
+        <v>8.9</v>
+      </c>
+      <c r="Q115" s="7">
+        <v>8.1</v>
+      </c>
+      <c r="R115" s="7">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B116">
+        <v>23</v>
+      </c>
+      <c r="C116" t="s">
+        <v>420</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="E116" t="s">
+        <v>133</v>
+      </c>
+      <c r="F116" t="s">
         <v>26</v>
       </c>
-      <c r="C116" t="s">
-        <v>420</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="E116" t="s">
-        <v>437</v>
-      </c>
-      <c r="F116" t="s">
-        <v>438</v>
-      </c>
       <c r="G116" t="s">
         <v>146</v>
       </c>
@@ -8519,13 +8437,13 @@
         <v>146</v>
       </c>
       <c r="I116" s="1">
-        <v>45355</v>
+        <v>45346</v>
       </c>
       <c r="J116" s="4">
-        <v>33.246605000000002</v>
+        <v>38.892167999999998</v>
       </c>
       <c r="K116" s="4">
-        <v>-111.84272</v>
+        <v>-77.025794000000005</v>
       </c>
       <c r="L116" s="6">
         <v>46</v>
@@ -8537,36 +8455,36 @@
         <v>1</v>
       </c>
       <c r="O116">
-        <v>18</v>
-      </c>
-      <c r="P116">
-        <v>2.25</v>
-      </c>
-      <c r="Q116">
-        <v>2.875</v>
-      </c>
-      <c r="R116">
-        <v>2.0625</v>
-      </c>
-    </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="P116" s="7">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="Q116" s="7">
+        <v>8.1</v>
+      </c>
+      <c r="R116" s="7">
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B117">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C117" t="s">
         <v>420</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>230</v>
+        <v>434</v>
       </c>
       <c r="E117" t="s">
-        <v>327</v>
+        <v>436</v>
       </c>
       <c r="F117" t="s">
-        <v>163</v>
+        <v>439</v>
       </c>
       <c r="G117" t="s">
         <v>146</v>
@@ -8575,13 +8493,13 @@
         <v>146</v>
       </c>
       <c r="I117" s="1">
-        <v>45311</v>
+        <v>45353</v>
       </c>
       <c r="J117" s="4">
-        <v>39.056086162518199</v>
+        <v>33.980536999999998</v>
       </c>
       <c r="K117" s="4">
-        <v>-77.114897400000004</v>
+        <v>-84.424716000000004</v>
       </c>
       <c r="L117" s="6">
         <v>46</v>
@@ -8593,37 +8511,36 @@
         <v>1</v>
       </c>
       <c r="O117">
-        <v>28</v>
-      </c>
-      <c r="P117">
-        <v>2.5</v>
-      </c>
-      <c r="Q117">
-        <f>2+6/16</f>
-        <v>2.375</v>
-      </c>
-      <c r="R117">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="P117" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="Q117" s="7">
+        <v>7.3</v>
+      </c>
+      <c r="R117" s="7">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="B118">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C118" t="s">
         <v>420</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>230</v>
+        <v>434</v>
       </c>
       <c r="E118" t="s">
-        <v>327</v>
+        <v>437</v>
       </c>
       <c r="F118" t="s">
-        <v>163</v>
+        <v>438</v>
       </c>
       <c r="G118" t="s">
         <v>146</v>
@@ -8632,13 +8549,13 @@
         <v>146</v>
       </c>
       <c r="I118" s="1">
-        <v>45311</v>
+        <v>45355</v>
       </c>
       <c r="J118" s="4">
-        <v>39.056086162518199</v>
+        <v>33.246605000000002</v>
       </c>
       <c r="K118" s="4">
-        <v>-77.114897400000004</v>
+        <v>-111.84272</v>
       </c>
       <c r="L118" s="6">
         <v>46</v>
@@ -8650,36 +8567,36 @@
         <v>1</v>
       </c>
       <c r="O118">
-        <v>28</v>
-      </c>
-      <c r="P118">
-        <v>2.75</v>
-      </c>
-      <c r="Q118">
-        <v>2.375</v>
-      </c>
-      <c r="R118">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="P118" s="7">
+        <v>7.1</v>
+      </c>
+      <c r="Q118" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="R118" s="7">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B119">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C119" t="s">
         <v>420</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E119" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="F119" t="s">
-        <v>165</v>
+        <v>438</v>
       </c>
       <c r="G119" t="s">
         <v>146</v>
@@ -8688,13 +8605,13 @@
         <v>146</v>
       </c>
       <c r="I119" s="1">
-        <v>45270</v>
+        <v>45355</v>
       </c>
       <c r="J119" s="4">
-        <v>42.787076999999996</v>
+        <v>33.246605000000002</v>
       </c>
       <c r="K119" s="4">
-        <v>-71.503960000000006</v>
+        <v>-111.84272</v>
       </c>
       <c r="L119" s="6">
         <v>46</v>
@@ -8703,24 +8620,22 @@
         <v>50</v>
       </c>
       <c r="N119">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O119">
-        <v>8</v>
-      </c>
-      <c r="P119">
-        <v>1.25</v>
-      </c>
-      <c r="Q119">
-        <f>1+7/16</f>
-        <v>1.4375</v>
-      </c>
-      <c r="R119">
-        <f>1+6/16</f>
-        <v>1.375</v>
-      </c>
-    </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="P119" s="7">
+        <v>5.7</v>
+      </c>
+      <c r="Q119" s="7">
+        <v>7.3</v>
+      </c>
+      <c r="R119" s="7">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>442</v>
       </c>
@@ -8766,19 +8681,17 @@
       <c r="O120">
         <v>28</v>
       </c>
-      <c r="P120">
-        <f>2+10/16</f>
-        <v>2.625</v>
-      </c>
-      <c r="Q120">
-        <v>2.25</v>
-      </c>
-      <c r="R120">
-        <f>2+15/16</f>
-        <v>2.9375</v>
-      </c>
-    </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P120" s="7">
+        <v>6.7</v>
+      </c>
+      <c r="Q120" s="7">
+        <v>5.7</v>
+      </c>
+      <c r="R120" s="7">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>443</v>
       </c>
@@ -8824,33 +8737,31 @@
       <c r="O121">
         <v>27</v>
       </c>
-      <c r="P121">
-        <v>2.25</v>
-      </c>
-      <c r="Q121">
-        <f>2+3/16</f>
-        <v>2.1875</v>
-      </c>
-      <c r="R121">
-        <f>2+6/16</f>
-        <v>2.375</v>
-      </c>
-    </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P121" s="7">
+        <v>5.7</v>
+      </c>
+      <c r="Q121" s="7">
+        <v>5.6</v>
+      </c>
+      <c r="R121" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B122">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C122" t="s">
-        <v>420</v>
+        <v>131</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="E122" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="F122" t="s">
         <v>167</v>
@@ -8862,43 +8773,42 @@
         <v>146</v>
       </c>
       <c r="I122" s="1">
-        <v>45407</v>
+        <v>45403</v>
       </c>
       <c r="J122" s="4">
-        <v>28.371808918683801</v>
+        <v>28.4809629890139</v>
       </c>
       <c r="K122" s="4">
-        <v>-81.517879136438097</v>
+        <v>-81.467406691372901</v>
       </c>
       <c r="L122" s="6">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M122" t="s">
         <v>50</v>
       </c>
       <c r="N122">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O122">
-        <v>18</v>
-      </c>
-      <c r="P122">
-        <v>2</v>
-      </c>
-      <c r="Q122">
-        <f>1+10/16</f>
-        <v>1.625</v>
-      </c>
-      <c r="R122">
-        <v>2.25</v>
-      </c>
-    </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="P122" s="7">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="Q122" s="7">
+        <v>5.4</v>
+      </c>
+      <c r="R122" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>445</v>
+        <v>241</v>
       </c>
       <c r="B123">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C123" t="s">
         <v>131</v>
@@ -8928,44 +8838,42 @@
         <v>-81.467406691372901</v>
       </c>
       <c r="L123" s="6">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M123" t="s">
         <v>50</v>
       </c>
       <c r="N123">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O123">
-        <v>35</v>
-      </c>
-      <c r="P123">
-        <f>1+10/16</f>
-        <v>1.625</v>
-      </c>
-      <c r="Q123">
-        <f>2+2/16</f>
-        <v>2.125</v>
-      </c>
-      <c r="R123">
-        <v>2.75</v>
-      </c>
-    </row>
-    <row r="124" spans="1:18" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="P123" s="7">
+        <v>5.9</v>
+      </c>
+      <c r="Q123" s="7">
+        <v>5.4</v>
+      </c>
+      <c r="R123" s="7">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>241</v>
+        <v>447</v>
       </c>
       <c r="B124">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C124" t="s">
-        <v>131</v>
+        <v>420</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>448</v>
+        <v>453</v>
       </c>
       <c r="E124" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="F124" t="s">
         <v>167</v>
@@ -8980,42 +8888,39 @@
         <v>45403</v>
       </c>
       <c r="J124" s="4">
-        <v>28.4809629890139</v>
+        <v>29.232650252891698</v>
       </c>
       <c r="K124" s="4">
-        <v>-81.467406691372901</v>
+        <v>-81.107395234459503</v>
       </c>
       <c r="L124" s="6">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="M124" t="s">
-        <v>50</v>
+        <v>449</v>
       </c>
       <c r="N124">
         <v>1</v>
       </c>
       <c r="O124">
-        <v>15</v>
-      </c>
-      <c r="P124">
-        <f>2+5/16</f>
-        <v>2.3125</v>
-      </c>
-      <c r="Q124">
-        <f>2+2/16</f>
-        <v>2.125</v>
-      </c>
-      <c r="R124">
-        <f>1+14/16</f>
-        <v>1.875</v>
-      </c>
-    </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="P124" s="7">
+        <v>7.6</v>
+      </c>
+      <c r="Q124" s="7">
+        <v>7</v>
+      </c>
+      <c r="R124" s="7">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B125">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C125" t="s">
         <v>420</v>
@@ -9024,7 +8929,7 @@
         <v>451</v>
       </c>
       <c r="E125" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="F125" t="s">
         <v>167</v>
@@ -9045,7 +8950,7 @@
         <v>-81.517879136438097</v>
       </c>
       <c r="L125" s="6">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="M125" t="s">
         <v>50</v>
@@ -9054,36 +8959,33 @@
         <v>1</v>
       </c>
       <c r="O125">
-        <v>14</v>
-      </c>
-      <c r="P125">
-        <f>2+2/16</f>
-        <v>2.125</v>
-      </c>
-      <c r="Q125">
-        <f>1+10/16</f>
-        <v>1.625</v>
-      </c>
-      <c r="R125">
-        <f>1+13/16</f>
-        <v>1.8125</v>
-      </c>
-    </row>
-    <row r="126" spans="1:18" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="P125" s="7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="Q125" s="7">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="R125" s="7">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="126" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B126">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C126" t="s">
         <v>420</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E126" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="F126" t="s">
         <v>167</v>
@@ -9095,41 +8997,40 @@
         <v>146</v>
       </c>
       <c r="I126" s="1">
-        <v>45403</v>
+        <v>45407</v>
       </c>
       <c r="J126" s="4">
-        <v>29.232650252891698</v>
+        <v>28.371808918683801</v>
       </c>
       <c r="K126" s="4">
-        <v>-81.107395234459503</v>
+        <v>-81.517879136438097</v>
       </c>
       <c r="L126" s="6">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M126" t="s">
-        <v>449</v>
+        <v>50</v>
       </c>
       <c r="N126">
         <v>1</v>
       </c>
       <c r="O126">
-        <v>48</v>
-      </c>
-      <c r="P126">
-        <v>3</v>
-      </c>
-      <c r="Q126">
-        <v>2.75</v>
-      </c>
-      <c r="R126">
-        <f>3+1/16</f>
-        <v>3.0625</v>
+        <v>14</v>
+      </c>
+      <c r="P126" s="7">
+        <v>5.4</v>
+      </c>
+      <c r="Q126" s="7">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="R126" s="7">
+        <v>4.5999999999999996</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="27" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -9144,20 +9045,20 @@
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>80</v>
       </c>
@@ -9186,13 +9087,13 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>80</v>
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -9209,7 +9110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -9226,43 +9127,43 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>73</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>74</v>
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>75</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>76</v>
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>77</v>
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>78</v>
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>79</v>
       </c>

</xml_diff>

<commit_message>
added rescue duck to db
</commit_message>
<xml_diff>
--- a/data/duck_data.xlsx
+++ b/data/duck_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\Documents\DS_Projects\portfolio-deployments\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C43914-BCB4-405D-9CD8-EDBD94FFB52A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397363FA-4186-4AE6-9E13-4DD028A2F0F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EF9DEEC2-186D-4161-AB80-57C24753F6AE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="456">
   <si>
     <t>Duck</t>
   </si>
@@ -1426,6 +1426,12 @@
   </si>
   <si>
     <t>Buc-ee's</t>
+  </si>
+  <si>
+    <t>Hawaiian</t>
+  </si>
+  <si>
+    <t>Disney Carribean Beach Resort</t>
   </si>
 </sst>
 </file>
@@ -1498,7 +1504,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1508,7 +1514,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1568,8 +1573,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55715085-9AFB-4516-817F-DC3F49C2B133}" name="Table1" displayName="Table1" ref="A1:R126" totalsRowShown="0">
-  <autoFilter ref="A1:R126" xr:uid="{55715085-9AFB-4516-817F-DC3F49C2B133}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{55715085-9AFB-4516-817F-DC3F49C2B133}" name="Table1" displayName="Table1" ref="A1:R127" totalsRowShown="0">
+  <autoFilter ref="A1:R127" xr:uid="{55715085-9AFB-4516-817F-DC3F49C2B133}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R126">
     <sortCondition ref="I1:I126"/>
   </sortState>
@@ -1915,12 +1920,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V126"/>
+  <dimension ref="A1:V127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A39" sqref="A39"/>
-      <selection pane="topRight" activeCell="L45" sqref="L45"/>
+      <selection pane="topRight" activeCell="R125" sqref="R125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4705,13 +4710,13 @@
       <c r="O49">
         <v>50</v>
       </c>
-      <c r="P49" s="7">
+      <c r="P49">
         <v>7.5</v>
       </c>
-      <c r="Q49" s="7">
+      <c r="Q49">
         <v>9.5</v>
       </c>
-      <c r="R49" s="7">
+      <c r="R49">
         <v>9.6999999999999993</v>
       </c>
     </row>
@@ -4761,13 +4766,13 @@
       <c r="O50">
         <v>47</v>
       </c>
-      <c r="P50" s="7">
+      <c r="P50">
         <v>7.6</v>
       </c>
-      <c r="Q50" s="7">
+      <c r="Q50">
         <v>9.8000000000000007</v>
       </c>
-      <c r="R50" s="7">
+      <c r="R50">
         <v>7.9</v>
       </c>
     </row>
@@ -4817,13 +4822,13 @@
       <c r="O51">
         <v>36</v>
       </c>
-      <c r="P51" s="7">
+      <c r="P51">
         <v>7.1</v>
       </c>
-      <c r="Q51" s="7">
+      <c r="Q51">
         <v>6</v>
       </c>
-      <c r="R51" s="7">
+      <c r="R51">
         <v>7.8</v>
       </c>
     </row>
@@ -4873,13 +4878,13 @@
       <c r="O52">
         <v>17</v>
       </c>
-      <c r="P52" s="7">
+      <c r="P52">
         <v>5.4</v>
       </c>
-      <c r="Q52" s="7">
+      <c r="Q52">
         <v>4.5</v>
       </c>
-      <c r="R52" s="7">
+      <c r="R52">
         <v>4.7</v>
       </c>
     </row>
@@ -4929,13 +4934,13 @@
       <c r="O53">
         <v>17</v>
       </c>
-      <c r="P53" s="7">
+      <c r="P53">
         <v>5.4</v>
       </c>
-      <c r="Q53" s="7">
+      <c r="Q53">
         <v>5.6</v>
       </c>
-      <c r="R53" s="7">
+      <c r="R53">
         <v>5.8</v>
       </c>
     </row>
@@ -4985,13 +4990,13 @@
       <c r="O54">
         <v>18</v>
       </c>
-      <c r="P54" s="7">
+      <c r="P54">
         <v>6.1</v>
       </c>
-      <c r="Q54" s="7">
+      <c r="Q54">
         <v>5.7</v>
       </c>
-      <c r="R54" s="7">
+      <c r="R54">
         <v>5.9</v>
       </c>
     </row>
@@ -5041,13 +5046,13 @@
       <c r="O55">
         <v>17</v>
       </c>
-      <c r="P55" s="7">
+      <c r="P55">
         <v>5.7</v>
       </c>
-      <c r="Q55" s="7">
+      <c r="Q55">
         <v>5.7</v>
       </c>
-      <c r="R55" s="7">
+      <c r="R55">
         <v>5.8</v>
       </c>
     </row>
@@ -5097,13 +5102,13 @@
       <c r="O56">
         <v>19</v>
       </c>
-      <c r="P56" s="7">
+      <c r="P56">
         <v>5.8</v>
       </c>
-      <c r="Q56" s="7">
+      <c r="Q56">
         <v>5.7</v>
       </c>
-      <c r="R56" s="7">
+      <c r="R56">
         <v>5.9</v>
       </c>
     </row>
@@ -5153,13 +5158,13 @@
       <c r="O57">
         <v>155</v>
       </c>
-      <c r="P57" s="7">
+      <c r="P57">
         <v>11.5</v>
       </c>
-      <c r="Q57" s="7">
+      <c r="Q57">
         <v>8.1</v>
       </c>
-      <c r="R57" s="7">
+      <c r="R57">
         <v>9.6999999999999993</v>
       </c>
     </row>
@@ -5209,13 +5214,13 @@
       <c r="O58">
         <v>9</v>
       </c>
-      <c r="P58" s="7">
+      <c r="P58">
         <v>3.3</v>
       </c>
-      <c r="Q58" s="7">
+      <c r="Q58">
         <v>4.7</v>
       </c>
-      <c r="R58" s="7">
+      <c r="R58">
         <v>5.4</v>
       </c>
     </row>
@@ -5265,13 +5270,13 @@
       <c r="O59">
         <v>11</v>
       </c>
-      <c r="P59" s="7">
+      <c r="P59">
         <v>6.4</v>
       </c>
-      <c r="Q59" s="7">
+      <c r="Q59">
         <v>3.3</v>
       </c>
-      <c r="R59" s="7">
+      <c r="R59">
         <v>4.3</v>
       </c>
     </row>
@@ -5321,13 +5326,13 @@
       <c r="O60">
         <v>145</v>
       </c>
-      <c r="P60" s="7">
+      <c r="P60">
         <v>7.3</v>
       </c>
-      <c r="Q60" s="7">
+      <c r="Q60">
         <v>6.4</v>
       </c>
-      <c r="R60" s="7">
+      <c r="R60">
         <v>8.3000000000000007</v>
       </c>
     </row>
@@ -5377,13 +5382,13 @@
       <c r="O61">
         <v>107</v>
       </c>
-      <c r="P61" s="7">
+      <c r="P61">
         <v>9.6999999999999993</v>
       </c>
-      <c r="Q61" s="7">
+      <c r="Q61">
         <v>8.3000000000000007</v>
       </c>
-      <c r="R61" s="7">
+      <c r="R61">
         <v>11.7</v>
       </c>
     </row>
@@ -5433,13 +5438,13 @@
       <c r="O62">
         <v>102</v>
       </c>
-      <c r="P62" s="7">
+      <c r="P62">
         <v>9.5</v>
       </c>
-      <c r="Q62" s="7">
+      <c r="Q62">
         <v>8.9</v>
       </c>
-      <c r="R62" s="7">
+      <c r="R62">
         <v>12.1</v>
       </c>
     </row>
@@ -5489,13 +5494,13 @@
       <c r="O63">
         <v>86</v>
       </c>
-      <c r="P63" s="7">
+      <c r="P63">
         <v>8.3000000000000007</v>
       </c>
-      <c r="Q63" s="7">
+      <c r="Q63">
         <v>7</v>
       </c>
-      <c r="R63" s="7">
+      <c r="R63">
         <v>9</v>
       </c>
     </row>
@@ -5545,13 +5550,13 @@
       <c r="O64">
         <v>18</v>
       </c>
-      <c r="P64" s="7">
+      <c r="P64">
         <v>5.0999999999999996</v>
       </c>
-      <c r="Q64" s="7">
+      <c r="Q64">
         <v>5.4</v>
       </c>
-      <c r="R64" s="7">
+      <c r="R64">
         <v>6.2</v>
       </c>
     </row>
@@ -5601,13 +5606,13 @@
       <c r="O65">
         <v>21</v>
       </c>
-      <c r="P65" s="7">
+      <c r="P65">
         <v>5.6</v>
       </c>
-      <c r="Q65" s="7">
+      <c r="Q65">
         <v>5.9</v>
       </c>
-      <c r="R65" s="7">
+      <c r="R65">
         <v>6.4</v>
       </c>
     </row>
@@ -5657,13 +5662,13 @@
       <c r="O66">
         <v>24</v>
       </c>
-      <c r="P66" s="7">
+      <c r="P66">
         <v>6.5</v>
       </c>
-      <c r="Q66" s="7">
+      <c r="Q66">
         <v>5.0999999999999996</v>
       </c>
-      <c r="R66" s="7">
+      <c r="R66">
         <v>5.7</v>
       </c>
     </row>
@@ -5713,13 +5718,13 @@
       <c r="O67">
         <v>26</v>
       </c>
-      <c r="P67" s="7">
+      <c r="P67">
         <v>6.7</v>
       </c>
-      <c r="Q67" s="7">
+      <c r="Q67">
         <v>5.7</v>
       </c>
-      <c r="R67" s="7">
+      <c r="R67">
         <v>5.6</v>
       </c>
     </row>
@@ -5769,13 +5774,13 @@
       <c r="O68">
         <v>162</v>
       </c>
-      <c r="P68" s="7">
+      <c r="P68">
         <v>13.3</v>
       </c>
-      <c r="Q68" s="7">
+      <c r="Q68">
         <v>13.7</v>
       </c>
-      <c r="R68" s="7">
+      <c r="R68">
         <v>16.5</v>
       </c>
     </row>
@@ -5825,13 +5830,13 @@
       <c r="O69">
         <v>25</v>
       </c>
-      <c r="P69" s="7">
+      <c r="P69">
         <v>7.5</v>
       </c>
-      <c r="Q69" s="7">
+      <c r="Q69">
         <v>5.4</v>
       </c>
-      <c r="R69" s="7">
+      <c r="R69">
         <v>5.4</v>
       </c>
     </row>
@@ -5881,13 +5886,13 @@
       <c r="O70">
         <v>24</v>
       </c>
-      <c r="P70" s="7">
+      <c r="P70">
         <v>6.7</v>
       </c>
-      <c r="Q70" s="7">
+      <c r="Q70">
         <v>4.9000000000000004</v>
       </c>
-      <c r="R70" s="7">
+      <c r="R70">
         <v>7.1</v>
       </c>
     </row>
@@ -5937,13 +5942,13 @@
       <c r="O71">
         <v>39</v>
       </c>
-      <c r="P71" s="7">
+      <c r="P71">
         <v>6.4</v>
       </c>
-      <c r="Q71" s="7">
+      <c r="Q71">
         <v>6.4</v>
       </c>
-      <c r="R71" s="7">
+      <c r="R71">
         <v>7.6</v>
       </c>
     </row>
@@ -5993,13 +5998,13 @@
       <c r="O72">
         <v>163</v>
       </c>
-      <c r="P72" s="7">
+      <c r="P72">
         <v>6.3</v>
       </c>
-      <c r="Q72" s="7">
+      <c r="Q72">
         <v>6.1</v>
       </c>
-      <c r="R72" s="7">
+      <c r="R72">
         <v>6.8</v>
       </c>
     </row>
@@ -6049,13 +6054,13 @@
       <c r="O73">
         <v>56</v>
       </c>
-      <c r="P73" s="7">
+      <c r="P73">
         <v>8.3000000000000007</v>
       </c>
-      <c r="Q73" s="7">
+      <c r="Q73">
         <v>7.9</v>
       </c>
-      <c r="R73" s="7">
+      <c r="R73">
         <v>8.9</v>
       </c>
     </row>
@@ -6105,13 +6110,13 @@
       <c r="O74">
         <v>56</v>
       </c>
-      <c r="P74" s="7">
+      <c r="P74">
         <v>8.3000000000000007</v>
       </c>
-      <c r="Q74" s="7">
+      <c r="Q74">
         <v>8.4</v>
       </c>
-      <c r="R74" s="7">
+      <c r="R74">
         <v>8.9</v>
       </c>
     </row>
@@ -6161,13 +6166,13 @@
       <c r="O75">
         <v>55</v>
       </c>
-      <c r="P75" s="7">
+      <c r="P75">
         <v>8.6</v>
       </c>
-      <c r="Q75" s="7">
+      <c r="Q75">
         <v>7.9</v>
       </c>
-      <c r="R75" s="7">
+      <c r="R75">
         <v>8.9</v>
       </c>
     </row>
@@ -6217,13 +6222,13 @@
       <c r="O76">
         <v>55</v>
       </c>
-      <c r="P76" s="7">
+      <c r="P76">
         <v>8.4</v>
       </c>
-      <c r="Q76" s="7">
+      <c r="Q76">
         <v>9.6999999999999993</v>
       </c>
-      <c r="R76" s="7">
+      <c r="R76">
         <v>9.1999999999999993</v>
       </c>
     </row>
@@ -6273,13 +6278,13 @@
       <c r="O77">
         <v>62</v>
       </c>
-      <c r="P77" s="7">
+      <c r="P77">
         <v>7.9</v>
       </c>
-      <c r="Q77" s="7">
+      <c r="Q77">
         <v>9.8000000000000007</v>
       </c>
-      <c r="R77" s="7">
+      <c r="R77">
         <v>8.9</v>
       </c>
     </row>
@@ -6329,13 +6334,13 @@
       <c r="O78">
         <v>116</v>
       </c>
-      <c r="P78" s="7">
+      <c r="P78">
         <v>7.9</v>
       </c>
-      <c r="Q78" s="7">
+      <c r="Q78">
         <v>6.7</v>
       </c>
-      <c r="R78" s="7">
+      <c r="R78">
         <v>8.9</v>
       </c>
     </row>
@@ -6385,13 +6390,13 @@
       <c r="O79">
         <v>67</v>
       </c>
-      <c r="P79" s="7">
+      <c r="P79">
         <v>11.3</v>
       </c>
-      <c r="Q79" s="7">
+      <c r="Q79">
         <v>7.8</v>
       </c>
-      <c r="R79" s="7">
+      <c r="R79">
         <v>10.3</v>
       </c>
     </row>
@@ -6441,13 +6446,13 @@
       <c r="O80">
         <v>59</v>
       </c>
-      <c r="P80" s="7">
+      <c r="P80">
         <v>9.6999999999999993</v>
       </c>
-      <c r="Q80" s="7">
+      <c r="Q80">
         <v>9.8000000000000007</v>
       </c>
-      <c r="R80" s="7">
+      <c r="R80">
         <v>8.6999999999999993</v>
       </c>
     </row>
@@ -6497,13 +6502,13 @@
       <c r="O81">
         <v>54</v>
       </c>
-      <c r="P81" s="7">
+      <c r="P81">
         <v>7.9</v>
       </c>
-      <c r="Q81" s="7">
+      <c r="Q81">
         <v>8.6999999999999993</v>
       </c>
-      <c r="R81" s="7">
+      <c r="R81">
         <v>12.2</v>
       </c>
     </row>
@@ -6553,13 +6558,13 @@
       <c r="O82">
         <v>95</v>
       </c>
-      <c r="P82" s="7">
+      <c r="P82">
         <v>7.8</v>
       </c>
-      <c r="Q82" s="7">
+      <c r="Q82">
         <v>12.4</v>
       </c>
-      <c r="R82" s="7">
+      <c r="R82">
         <v>12.4</v>
       </c>
     </row>
@@ -6609,13 +6614,13 @@
       <c r="O83">
         <v>0.1</v>
       </c>
-      <c r="P83" s="7">
+      <c r="P83">
         <v>1.6</v>
       </c>
-      <c r="Q83" s="7">
+      <c r="Q83">
         <v>1.4</v>
       </c>
-      <c r="R83" s="7">
+      <c r="R83">
         <v>1.4</v>
       </c>
     </row>
@@ -6665,13 +6670,13 @@
       <c r="O84">
         <v>42</v>
       </c>
-      <c r="P84" s="7">
+      <c r="P84">
         <v>9.8000000000000007</v>
       </c>
-      <c r="Q84" s="7">
+      <c r="Q84">
         <v>9.4</v>
       </c>
-      <c r="R84" s="7">
+      <c r="R84">
         <v>8.3000000000000007</v>
       </c>
     </row>
@@ -6721,13 +6726,13 @@
       <c r="O85">
         <v>48</v>
       </c>
-      <c r="P85" s="7">
+      <c r="P85">
         <v>8.4</v>
       </c>
-      <c r="Q85" s="7">
+      <c r="Q85">
         <v>9.5</v>
       </c>
-      <c r="R85" s="7">
+      <c r="R85">
         <v>9.1999999999999993</v>
       </c>
     </row>
@@ -6777,13 +6782,13 @@
       <c r="O86">
         <v>66</v>
       </c>
-      <c r="P86" s="7">
+      <c r="P86">
         <v>7.1</v>
       </c>
-      <c r="Q86" s="7">
+      <c r="Q86">
         <v>7.3</v>
       </c>
-      <c r="R86" s="7">
+      <c r="R86">
         <v>8.4</v>
       </c>
     </row>
@@ -6833,13 +6838,13 @@
       <c r="O87">
         <v>22</v>
       </c>
-      <c r="P87" s="7">
+      <c r="P87">
         <v>6.8</v>
       </c>
-      <c r="Q87" s="7">
+      <c r="Q87">
         <v>5.0999999999999996</v>
       </c>
-      <c r="R87" s="7">
+      <c r="R87">
         <v>5.6</v>
       </c>
     </row>
@@ -6889,13 +6894,13 @@
       <c r="O88">
         <v>17</v>
       </c>
-      <c r="P88" s="7">
+      <c r="P88">
         <v>4</v>
       </c>
-      <c r="Q88" s="7">
+      <c r="Q88">
         <v>4.4000000000000004</v>
       </c>
-      <c r="R88" s="7">
+      <c r="R88">
         <v>4.5999999999999996</v>
       </c>
     </row>
@@ -6945,13 +6950,13 @@
       <c r="O89">
         <v>19</v>
       </c>
-      <c r="P89" s="7">
+      <c r="P89">
         <v>6</v>
       </c>
-      <c r="Q89" s="7">
+      <c r="Q89">
         <v>4.8</v>
       </c>
-      <c r="R89" s="7">
+      <c r="R89">
         <v>6.2</v>
       </c>
     </row>
@@ -7001,13 +7006,13 @@
       <c r="O90">
         <v>15</v>
       </c>
-      <c r="P90" s="7">
+      <c r="P90">
         <v>7.3</v>
       </c>
-      <c r="Q90" s="7">
+      <c r="Q90">
         <v>5.0999999999999996</v>
       </c>
-      <c r="R90" s="7">
+      <c r="R90">
         <v>5.0999999999999996</v>
       </c>
     </row>
@@ -7057,13 +7062,13 @@
       <c r="O91">
         <v>18</v>
       </c>
-      <c r="P91" s="7">
+      <c r="P91">
         <v>6.2</v>
       </c>
-      <c r="Q91" s="7">
+      <c r="Q91">
         <v>4.9000000000000004</v>
       </c>
-      <c r="R91" s="7">
+      <c r="R91">
         <v>3.5</v>
       </c>
     </row>
@@ -7113,13 +7118,13 @@
       <c r="O92">
         <v>17</v>
       </c>
-      <c r="P92" s="7">
+      <c r="P92">
         <v>4.9000000000000004</v>
       </c>
-      <c r="Q92" s="7">
+      <c r="Q92">
         <v>4.8</v>
       </c>
-      <c r="R92" s="7">
+      <c r="R92">
         <v>5.0999999999999996</v>
       </c>
     </row>
@@ -7169,13 +7174,13 @@
       <c r="O93">
         <v>14</v>
       </c>
-      <c r="P93" s="7">
+      <c r="P93">
         <v>4.9000000000000004</v>
       </c>
-      <c r="Q93" s="7">
+      <c r="Q93">
         <v>4.5999999999999996</v>
       </c>
-      <c r="R93" s="7">
+      <c r="R93">
         <v>4.8</v>
       </c>
     </row>
@@ -7225,13 +7230,13 @@
       <c r="O94">
         <v>6</v>
       </c>
-      <c r="P94" s="7">
+      <c r="P94">
         <v>2.9</v>
       </c>
-      <c r="Q94" s="7">
+      <c r="Q94">
         <v>3.7</v>
       </c>
-      <c r="R94" s="7">
+      <c r="R94">
         <v>3.3</v>
       </c>
     </row>
@@ -7281,13 +7286,13 @@
       <c r="O95">
         <v>43</v>
       </c>
-      <c r="P95" s="7">
+      <c r="P95">
         <v>7.6</v>
       </c>
-      <c r="Q95" s="7">
+      <c r="Q95">
         <v>7.3</v>
       </c>
-      <c r="R95" s="7">
+      <c r="R95">
         <v>8.4</v>
       </c>
     </row>
@@ -7337,13 +7342,13 @@
       <c r="O96">
         <v>45</v>
       </c>
-      <c r="P96" s="7">
+      <c r="P96">
         <v>8.4</v>
       </c>
-      <c r="Q96" s="7">
+      <c r="Q96">
         <v>9.8000000000000007</v>
       </c>
-      <c r="R96" s="7">
+      <c r="R96">
         <v>7.9</v>
       </c>
     </row>
@@ -7393,13 +7398,13 @@
       <c r="O97">
         <v>48</v>
       </c>
-      <c r="P97" s="7">
+      <c r="P97">
         <v>8.6</v>
       </c>
-      <c r="Q97" s="7">
+      <c r="Q97">
         <v>9.8000000000000007</v>
       </c>
-      <c r="R97" s="7">
+      <c r="R97">
         <v>7.9</v>
       </c>
     </row>
@@ -7449,13 +7454,13 @@
       <c r="O98">
         <v>47</v>
       </c>
-      <c r="P98" s="7">
+      <c r="P98">
         <v>8.6</v>
       </c>
-      <c r="Q98" s="7">
+      <c r="Q98">
         <v>9.8000000000000007</v>
       </c>
-      <c r="R98" s="7">
+      <c r="R98">
         <v>7.9</v>
       </c>
     </row>
@@ -7505,13 +7510,13 @@
       <c r="O99">
         <v>153</v>
       </c>
-      <c r="P99" s="7">
+      <c r="P99">
         <v>12.7</v>
       </c>
-      <c r="Q99" s="7">
+      <c r="Q99">
         <v>13.3</v>
       </c>
-      <c r="R99" s="7">
+      <c r="R99">
         <v>16.5</v>
       </c>
     </row>
@@ -7561,13 +7566,13 @@
       <c r="O100">
         <v>19</v>
       </c>
-      <c r="P100" s="7">
+      <c r="P100">
         <v>4.9000000000000004</v>
       </c>
-      <c r="Q100" s="7">
+      <c r="Q100">
         <v>4.8</v>
       </c>
-      <c r="R100" s="7">
+      <c r="R100">
         <v>5.9</v>
       </c>
     </row>
@@ -7617,13 +7622,13 @@
       <c r="O101">
         <v>19</v>
       </c>
-      <c r="P101" s="7">
+      <c r="P101">
         <v>5.0999999999999996</v>
       </c>
-      <c r="Q101" s="7">
+      <c r="Q101">
         <v>4.8</v>
       </c>
-      <c r="R101" s="7">
+      <c r="R101">
         <v>5.9</v>
       </c>
     </row>
@@ -7673,13 +7678,13 @@
       <c r="O102">
         <v>18</v>
       </c>
-      <c r="P102" s="7">
+      <c r="P102">
         <v>5.0999999999999996</v>
       </c>
-      <c r="Q102" s="7">
+      <c r="Q102">
         <v>4.8</v>
       </c>
-      <c r="R102" s="7">
+      <c r="R102">
         <v>5.6</v>
       </c>
     </row>
@@ -7729,13 +7734,13 @@
       <c r="O103">
         <v>18</v>
       </c>
-      <c r="P103" s="7">
+      <c r="P103">
         <v>5.2</v>
       </c>
-      <c r="Q103" s="7">
+      <c r="Q103">
         <v>4.8</v>
       </c>
-      <c r="R103" s="7">
+      <c r="R103">
         <v>5.4</v>
       </c>
     </row>
@@ -7785,13 +7790,13 @@
       <c r="O104">
         <v>22</v>
       </c>
-      <c r="P104" s="7">
+      <c r="P104">
         <v>6.4</v>
       </c>
-      <c r="Q104" s="7">
+      <c r="Q104">
         <v>4.9000000000000004</v>
       </c>
-      <c r="R104" s="7">
+      <c r="R104">
         <v>5.4</v>
       </c>
     </row>
@@ -7841,13 +7846,13 @@
       <c r="O105">
         <v>20</v>
       </c>
-      <c r="P105" s="7">
+      <c r="P105">
         <v>5.9</v>
       </c>
-      <c r="Q105" s="7">
+      <c r="Q105">
         <v>4.3</v>
       </c>
-      <c r="R105" s="7">
+      <c r="R105">
         <v>6.2</v>
       </c>
     </row>
@@ -7897,13 +7902,13 @@
       <c r="O106">
         <v>70</v>
       </c>
-      <c r="P106" s="7">
+      <c r="P106">
         <v>6.7</v>
       </c>
-      <c r="Q106" s="7">
+      <c r="Q106">
         <v>7.6</v>
       </c>
-      <c r="R106" s="7">
+      <c r="R106">
         <v>6.7</v>
       </c>
     </row>
@@ -7953,13 +7958,13 @@
       <c r="O107">
         <v>17</v>
       </c>
-      <c r="P107" s="7">
+      <c r="P107">
         <v>5.7</v>
       </c>
-      <c r="Q107" s="7">
+      <c r="Q107">
         <v>4.8</v>
       </c>
-      <c r="R107" s="7">
+      <c r="R107">
         <v>4.8</v>
       </c>
     </row>
@@ -8009,13 +8014,13 @@
       <c r="O108">
         <v>15</v>
       </c>
-      <c r="P108" s="7">
+      <c r="P108">
         <v>5.0999999999999996</v>
       </c>
-      <c r="Q108" s="7">
+      <c r="Q108">
         <v>4.5999999999999996</v>
       </c>
-      <c r="R108" s="7">
+      <c r="R108">
         <v>4.8</v>
       </c>
     </row>
@@ -8065,13 +8070,13 @@
       <c r="O109">
         <v>54</v>
       </c>
-      <c r="P109" s="7">
+      <c r="P109">
         <v>7.6</v>
       </c>
-      <c r="Q109" s="7">
+      <c r="Q109">
         <v>6.7</v>
       </c>
-      <c r="R109" s="7">
+      <c r="R109">
         <v>8.9</v>
       </c>
     </row>
@@ -8121,13 +8126,13 @@
       <c r="O110">
         <v>17</v>
       </c>
-      <c r="P110" s="7">
+      <c r="P110">
         <v>4.4000000000000004</v>
       </c>
-      <c r="Q110" s="7">
+      <c r="Q110">
         <v>4.5999999999999996</v>
       </c>
-      <c r="R110" s="7">
+      <c r="R110">
         <v>5.0999999999999996</v>
       </c>
     </row>
@@ -8177,13 +8182,13 @@
       <c r="O111">
         <v>68</v>
       </c>
-      <c r="P111" s="7">
+      <c r="P111">
         <v>8.9</v>
       </c>
-      <c r="Q111" s="7">
+      <c r="Q111">
         <v>8.6</v>
       </c>
-      <c r="R111" s="7">
+      <c r="R111">
         <v>9</v>
       </c>
     </row>
@@ -8233,13 +8238,13 @@
       <c r="O112">
         <v>8</v>
       </c>
-      <c r="P112" s="7">
+      <c r="P112">
         <v>3.2</v>
       </c>
-      <c r="Q112" s="7">
+      <c r="Q112">
         <v>3.7</v>
       </c>
-      <c r="R112" s="7">
+      <c r="R112">
         <v>3.5</v>
       </c>
     </row>
@@ -8289,13 +8294,13 @@
       <c r="O113">
         <v>28</v>
       </c>
-      <c r="P113" s="7">
+      <c r="P113">
         <v>6.4</v>
       </c>
-      <c r="Q113" s="7">
+      <c r="Q113">
         <v>6</v>
       </c>
-      <c r="R113" s="7">
+      <c r="R113">
         <v>6.4</v>
       </c>
     </row>
@@ -8345,13 +8350,13 @@
       <c r="O114">
         <v>28</v>
       </c>
-      <c r="P114" s="7">
+      <c r="P114">
         <v>7</v>
       </c>
-      <c r="Q114" s="7">
+      <c r="Q114">
         <v>6</v>
       </c>
-      <c r="R114" s="7">
+      <c r="R114">
         <v>7.6</v>
       </c>
     </row>
@@ -8401,13 +8406,13 @@
       <c r="O115">
         <v>65</v>
       </c>
-      <c r="P115" s="7">
+      <c r="P115">
         <v>8.9</v>
       </c>
-      <c r="Q115" s="7">
+      <c r="Q115">
         <v>8.1</v>
       </c>
-      <c r="R115" s="7">
+      <c r="R115">
         <v>10.6</v>
       </c>
     </row>
@@ -8457,13 +8462,13 @@
       <c r="O116">
         <v>64</v>
       </c>
-      <c r="P116" s="7">
+      <c r="P116">
         <v>8.3000000000000007</v>
       </c>
-      <c r="Q116" s="7">
+      <c r="Q116">
         <v>8.1</v>
       </c>
-      <c r="R116" s="7">
+      <c r="R116">
         <v>12.4</v>
       </c>
     </row>
@@ -8513,13 +8518,13 @@
       <c r="O117">
         <v>16</v>
       </c>
-      <c r="P117" s="7">
+      <c r="P117">
         <v>5.0999999999999996</v>
       </c>
-      <c r="Q117" s="7">
+      <c r="Q117">
         <v>7.3</v>
       </c>
-      <c r="R117" s="7">
+      <c r="R117">
         <v>5.2</v>
       </c>
     </row>
@@ -8569,13 +8574,13 @@
       <c r="O118">
         <v>18</v>
       </c>
-      <c r="P118" s="7">
+      <c r="P118">
         <v>7.1</v>
       </c>
-      <c r="Q118" s="7">
+      <c r="Q118">
         <v>5.0999999999999996</v>
       </c>
-      <c r="R118" s="7">
+      <c r="R118">
         <v>5.2</v>
       </c>
     </row>
@@ -8625,13 +8630,13 @@
       <c r="O119">
         <v>18</v>
       </c>
-      <c r="P119" s="7">
+      <c r="P119">
         <v>5.7</v>
       </c>
-      <c r="Q119" s="7">
+      <c r="Q119">
         <v>7.3</v>
       </c>
-      <c r="R119" s="7">
+      <c r="R119">
         <v>5.2</v>
       </c>
     </row>
@@ -8681,13 +8686,13 @@
       <c r="O120">
         <v>28</v>
       </c>
-      <c r="P120" s="7">
+      <c r="P120">
         <v>6.7</v>
       </c>
-      <c r="Q120" s="7">
+      <c r="Q120">
         <v>5.7</v>
       </c>
-      <c r="R120" s="7">
+      <c r="R120">
         <v>7.5</v>
       </c>
     </row>
@@ -8737,13 +8742,13 @@
       <c r="O121">
         <v>27</v>
       </c>
-      <c r="P121" s="7">
+      <c r="P121">
         <v>5.7</v>
       </c>
-      <c r="Q121" s="7">
+      <c r="Q121">
         <v>5.6</v>
       </c>
-      <c r="R121" s="7">
+      <c r="R121">
         <v>6</v>
       </c>
     </row>
@@ -8793,13 +8798,13 @@
       <c r="O122">
         <v>35</v>
       </c>
-      <c r="P122" s="7">
+      <c r="P122">
         <v>4.0999999999999996</v>
       </c>
-      <c r="Q122" s="7">
+      <c r="Q122">
         <v>5.4</v>
       </c>
-      <c r="R122" s="7">
+      <c r="R122">
         <v>7</v>
       </c>
     </row>
@@ -8849,13 +8854,13 @@
       <c r="O123">
         <v>15</v>
       </c>
-      <c r="P123" s="7">
+      <c r="P123">
         <v>5.9</v>
       </c>
-      <c r="Q123" s="7">
+      <c r="Q123">
         <v>5.4</v>
       </c>
-      <c r="R123" s="7">
+      <c r="R123">
         <v>4.8</v>
       </c>
     </row>
@@ -8905,13 +8910,13 @@
       <c r="O124">
         <v>48</v>
       </c>
-      <c r="P124" s="7">
+      <c r="P124">
         <v>7.6</v>
       </c>
-      <c r="Q124" s="7">
+      <c r="Q124">
         <v>7</v>
       </c>
-      <c r="R124" s="7">
+      <c r="R124">
         <v>7.8</v>
       </c>
     </row>
@@ -8961,13 +8966,13 @@
       <c r="O125">
         <v>18</v>
       </c>
-      <c r="P125" s="7">
+      <c r="P125">
         <v>5.0999999999999996</v>
       </c>
-      <c r="Q125" s="7">
+      <c r="Q125">
         <v>4.0999999999999996</v>
       </c>
-      <c r="R125" s="7">
+      <c r="R125">
         <v>5.7</v>
       </c>
     </row>
@@ -9017,14 +9022,70 @@
       <c r="O126">
         <v>14</v>
       </c>
-      <c r="P126" s="7">
+      <c r="P126">
         <v>5.4</v>
       </c>
-      <c r="Q126" s="7">
+      <c r="Q126">
         <v>4.0999999999999996</v>
       </c>
-      <c r="R126" s="7">
+      <c r="R126">
         <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="127" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>454</v>
+      </c>
+      <c r="B127">
+        <v>60</v>
+      </c>
+      <c r="C127" t="s">
+        <v>98</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="E127" t="s">
+        <v>452</v>
+      </c>
+      <c r="F127" t="s">
+        <v>167</v>
+      </c>
+      <c r="G127" t="s">
+        <v>146</v>
+      </c>
+      <c r="H127" t="s">
+        <v>146</v>
+      </c>
+      <c r="I127" s="1">
+        <v>45405</v>
+      </c>
+      <c r="J127" s="4">
+        <v>28.3616867683712</v>
+      </c>
+      <c r="K127" s="4">
+        <v>-81.544157111972098</v>
+      </c>
+      <c r="L127" s="6">
+        <v>52</v>
+      </c>
+      <c r="M127" t="s">
+        <v>449</v>
+      </c>
+      <c r="N127">
+        <v>1</v>
+      </c>
+      <c r="O127">
+        <v>19</v>
+      </c>
+      <c r="P127">
+        <v>5</v>
+      </c>
+      <c r="Q127">
+        <v>5.3</v>
+      </c>
+      <c r="R127">
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>